<commit_message>
Progress on Data Pre-Processing.
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26760" windowHeight="11070" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26760" windowHeight="11070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Building" sheetId="1" r:id="rId1"/>
@@ -251,12 +251,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -594,7 +591,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,63 +612,63 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="9"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -692,7 +689,7 @@
       <c r="F5">
         <v>1993</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>14000</v>
       </c>
       <c r="I5" t="s">
@@ -718,7 +715,7 @@
       <c r="F6">
         <v>1990</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>23000</v>
       </c>
       <c r="I6" t="s">
@@ -734,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,15 +748,15 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>39083</v>
       </c>
       <c r="B5">
@@ -767,7 +764,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>39114</v>
       </c>
       <c r="B6">
@@ -775,7 +772,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>39142</v>
       </c>
       <c r="B7">
@@ -783,7 +780,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>39173</v>
       </c>
       <c r="B8">
@@ -791,7 +788,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>39203</v>
       </c>
       <c r="B9">
@@ -799,7 +796,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>39234</v>
       </c>
       <c r="B10">
@@ -807,7 +804,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <v>39264</v>
       </c>
       <c r="B11">
@@ -815,7 +812,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="10">
         <v>39295</v>
       </c>
       <c r="B12">
@@ -823,7 +820,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="10">
         <v>39326</v>
       </c>
       <c r="B13">
@@ -831,7 +828,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11">
+      <c r="A14" s="10">
         <v>39356</v>
       </c>
       <c r="B14">
@@ -839,7 +836,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11">
+      <c r="A15" s="10">
         <v>39387</v>
       </c>
       <c r="B15">
@@ -847,7 +844,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
+      <c r="A16" s="10">
         <v>39417</v>
       </c>
       <c r="B16">
@@ -855,7 +852,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
+      <c r="A17" s="10">
         <v>39448</v>
       </c>
       <c r="B17">
@@ -863,7 +860,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11">
+      <c r="A18" s="10">
         <v>39479</v>
       </c>
       <c r="B18">
@@ -871,7 +868,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="11">
+      <c r="A19" s="10">
         <v>39508</v>
       </c>
       <c r="B19">
@@ -879,7 +876,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>39539</v>
       </c>
       <c r="B20">
@@ -887,7 +884,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11">
+      <c r="A21" s="10">
         <v>39569</v>
       </c>
       <c r="B21">
@@ -895,7 +892,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="10">
         <v>39600</v>
       </c>
       <c r="B22">
@@ -903,7 +900,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="10">
         <v>39630</v>
       </c>
       <c r="B23">
@@ -911,7 +908,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+      <c r="A24" s="10">
         <v>39661</v>
       </c>
       <c r="B24">
@@ -919,7 +916,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="A25" s="10">
         <v>39692</v>
       </c>
       <c r="B25">
@@ -927,7 +924,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="10">
         <v>39722</v>
       </c>
       <c r="B26">
@@ -935,7 +932,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="A27" s="10">
         <v>39753</v>
       </c>
       <c r="B27">
@@ -943,7 +940,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="10">
         <v>39783</v>
       </c>
       <c r="B28">
@@ -951,7 +948,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="A29" s="10">
         <v>39814</v>
       </c>
       <c r="B29">
@@ -959,7 +956,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+      <c r="A30" s="10">
         <v>39845</v>
       </c>
       <c r="B30">
@@ -967,7 +964,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+      <c r="A31" s="10">
         <v>39873</v>
       </c>
       <c r="B31">
@@ -975,7 +972,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+      <c r="A32" s="10">
         <v>39904</v>
       </c>
       <c r="B32">
@@ -983,7 +980,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+      <c r="A33" s="10">
         <v>39934</v>
       </c>
       <c r="B33">
@@ -991,7 +988,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+      <c r="A34" s="10">
         <v>39965</v>
       </c>
       <c r="B34">
@@ -999,7 +996,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+      <c r="A35" s="10">
         <v>39995</v>
       </c>
       <c r="B35">
@@ -1007,7 +1004,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+      <c r="A36" s="10">
         <v>40026</v>
       </c>
       <c r="B36">
@@ -1015,7 +1012,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+      <c r="A37" s="10">
         <v>40057</v>
       </c>
       <c r="B37">
@@ -1023,7 +1020,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="A38" s="10">
         <v>40087</v>
       </c>
       <c r="B38">
@@ -1031,7 +1028,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="A39" s="10">
         <v>40118</v>
       </c>
       <c r="B39">
@@ -1039,7 +1036,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="A40" s="10">
         <v>40148</v>
       </c>
       <c r="B40">
@@ -1047,7 +1044,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="A41" s="10">
         <v>40179</v>
       </c>
       <c r="B41">
@@ -1055,7 +1052,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+      <c r="A42" s="10">
         <v>40210</v>
       </c>
       <c r="B42">
@@ -1063,7 +1060,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11">
+      <c r="A43" s="10">
         <v>40238</v>
       </c>
       <c r="B43">
@@ -1071,7 +1068,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+      <c r="A44" s="10">
         <v>40269</v>
       </c>
       <c r="B44">
@@ -1079,7 +1076,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+      <c r="A45" s="10">
         <v>40299</v>
       </c>
       <c r="B45">
@@ -1087,7 +1084,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+      <c r="A46" s="10">
         <v>40330</v>
       </c>
       <c r="B46">
@@ -1095,7 +1092,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+      <c r="A47" s="10">
         <v>40360</v>
       </c>
       <c r="B47">
@@ -1103,7 +1100,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
+      <c r="A48" s="10">
         <v>40391</v>
       </c>
       <c r="B48">
@@ -1111,7 +1108,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+      <c r="A49" s="10">
         <v>40422</v>
       </c>
       <c r="B49">
@@ -1119,7 +1116,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+      <c r="A50" s="10">
         <v>40452</v>
       </c>
       <c r="B50">
@@ -1127,7 +1124,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
+      <c r="A51" s="10">
         <v>40483</v>
       </c>
       <c r="B51">
@@ -1135,7 +1132,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
+      <c r="A52" s="10">
         <v>40513</v>
       </c>
       <c r="B52">
@@ -1143,7 +1140,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
+      <c r="A53" s="10">
         <v>40544</v>
       </c>
       <c r="B53">
@@ -1151,7 +1148,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="11">
+      <c r="A54" s="10">
         <v>40575</v>
       </c>
       <c r="B54">
@@ -1159,7 +1156,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="11">
+      <c r="A55" s="10">
         <v>40603</v>
       </c>
       <c r="B55">
@@ -1167,7 +1164,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="11">
+      <c r="A56" s="10">
         <v>40634</v>
       </c>
       <c r="B56">
@@ -1175,7 +1172,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="11">
+      <c r="A57" s="10">
         <v>40664</v>
       </c>
       <c r="B57">
@@ -1183,7 +1180,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="11">
+      <c r="A58" s="10">
         <v>40695</v>
       </c>
       <c r="B58">
@@ -1191,7 +1188,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="11">
+      <c r="A59" s="10">
         <v>40725</v>
       </c>
       <c r="B59">
@@ -1199,7 +1196,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="11">
+      <c r="A60" s="10">
         <v>40756</v>
       </c>
       <c r="B60">
@@ -1207,7 +1204,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="11">
+      <c r="A61" s="10">
         <v>40787</v>
       </c>
       <c r="B61">
@@ -1215,7 +1212,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="11">
+      <c r="A62" s="10">
         <v>40817</v>
       </c>
       <c r="B62">
@@ -1223,7 +1220,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="11">
+      <c r="A63" s="10">
         <v>40848</v>
       </c>
       <c r="B63">
@@ -1231,7 +1228,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="11">
+      <c r="A64" s="10">
         <v>40878</v>
       </c>
       <c r="B64">
@@ -1239,7 +1236,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11">
+      <c r="A65" s="10">
         <v>40909</v>
       </c>
       <c r="B65">
@@ -1247,7 +1244,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="11">
+      <c r="A66" s="10">
         <v>40940</v>
       </c>
       <c r="B66">
@@ -1255,7 +1252,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="11">
+      <c r="A67" s="10">
         <v>40969</v>
       </c>
       <c r="B67">
@@ -1263,7 +1260,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="11">
+      <c r="A68" s="10">
         <v>41000</v>
       </c>
       <c r="B68">
@@ -1271,7 +1268,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11">
+      <c r="A69" s="10">
         <v>41030</v>
       </c>
       <c r="B69">
@@ -1279,7 +1276,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="11">
+      <c r="A70" s="10">
         <v>41061</v>
       </c>
       <c r="B70">
@@ -1287,7 +1284,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="11">
+      <c r="A71" s="10">
         <v>41091</v>
       </c>
       <c r="B71">
@@ -1295,7 +1292,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="11">
+      <c r="A72" s="10">
         <v>41122</v>
       </c>
       <c r="B72">
@@ -1303,7 +1300,7 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="11">
+      <c r="A73" s="10">
         <v>41153</v>
       </c>
       <c r="B73">
@@ -1311,7 +1308,7 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="11">
+      <c r="A74" s="10">
         <v>41183</v>
       </c>
       <c r="B74">
@@ -1319,7 +1316,7 @@
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="11">
+      <c r="A75" s="10">
         <v>41214</v>
       </c>
       <c r="B75">
@@ -1327,7 +1324,7 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="11">
+      <c r="A76" s="10">
         <v>41244</v>
       </c>
       <c r="B76">
@@ -1335,7 +1332,7 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="11">
+      <c r="A77" s="10">
         <v>41275</v>
       </c>
       <c r="B77">
@@ -1343,7 +1340,7 @@
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="11">
+      <c r="A78" s="10">
         <v>41306</v>
       </c>
       <c r="B78">
@@ -1351,7 +1348,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="11">
+      <c r="A79" s="10">
         <v>41334</v>
       </c>
       <c r="B79">
@@ -1359,7 +1356,7 @@
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="11">
+      <c r="A80" s="10">
         <v>41365</v>
       </c>
       <c r="B80">
@@ -1367,7 +1364,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="11">
+      <c r="A81" s="10">
         <v>41395</v>
       </c>
       <c r="B81">
@@ -1375,7 +1372,7 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="11">
+      <c r="A82" s="10">
         <v>41426</v>
       </c>
       <c r="B82">
@@ -1383,7 +1380,7 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="11">
+      <c r="A83" s="10">
         <v>41456</v>
       </c>
       <c r="B83">
@@ -1391,7 +1388,7 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="11">
+      <c r="A84" s="10">
         <v>41487</v>
       </c>
       <c r="B84">
@@ -1399,7 +1396,7 @@
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="11">
+      <c r="A85" s="10">
         <v>41518</v>
       </c>
       <c r="B85">
@@ -1407,7 +1404,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="11">
+      <c r="A86" s="10">
         <v>41548</v>
       </c>
       <c r="B86">
@@ -1415,7 +1412,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="11">
+      <c r="A87" s="10">
         <v>41579</v>
       </c>
       <c r="B87">
@@ -1423,7 +1420,7 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="11">
+      <c r="A88" s="10">
         <v>41609</v>
       </c>
       <c r="B88">
@@ -1431,7 +1428,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="11">
+      <c r="A89" s="10">
         <v>41640</v>
       </c>
       <c r="B89">
@@ -1439,7 +1436,7 @@
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="11">
+      <c r="A90" s="10">
         <v>41671</v>
       </c>
       <c r="B90">
@@ -1447,7 +1444,7 @@
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="11">
+      <c r="A91" s="10">
         <v>41699</v>
       </c>
       <c r="B91">
@@ -1455,7 +1452,7 @@
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="11">
+      <c r="A92" s="10">
         <v>41730</v>
       </c>
       <c r="B92">
@@ -1463,7 +1460,7 @@
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="11">
+      <c r="A93" s="10">
         <v>41760</v>
       </c>
       <c r="B93">
@@ -1471,7 +1468,7 @@
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="11">
+      <c r="A94" s="10">
         <v>41791</v>
       </c>
       <c r="B94">
@@ -1479,7 +1476,7 @@
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="11">
+      <c r="A95" s="10">
         <v>41821</v>
       </c>
       <c r="B95">
@@ -1487,7 +1484,7 @@
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="11">
+      <c r="A96" s="10">
         <v>41852</v>
       </c>
       <c r="B96">
@@ -1495,7 +1492,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="11">
+      <c r="A97" s="10">
         <v>41883</v>
       </c>
       <c r="B97">
@@ -1503,7 +1500,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="11">
+      <c r="A98" s="10">
         <v>41913</v>
       </c>
       <c r="B98">
@@ -1511,7 +1508,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="11">
+      <c r="A99" s="10">
         <v>41944</v>
       </c>
       <c r="B99">
@@ -1519,7 +1516,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="11">
+      <c r="A100" s="10">
         <v>41974</v>
       </c>
       <c r="B100">
@@ -1527,7 +1524,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="11">
+      <c r="A101" s="10">
         <v>42005</v>
       </c>
       <c r="B101">
@@ -1535,7 +1532,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="11">
+      <c r="A102" s="10">
         <v>42036</v>
       </c>
       <c r="B102">
@@ -1543,7 +1540,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="11">
+      <c r="A103" s="10">
         <v>42064</v>
       </c>
       <c r="B103">
@@ -1551,7 +1548,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="11">
+      <c r="A104" s="10">
         <v>42095</v>
       </c>
       <c r="B104">
@@ -1559,7 +1556,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="11">
+      <c r="A105" s="10">
         <v>42125</v>
       </c>
       <c r="B105">
@@ -1567,7 +1564,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="11">
+      <c r="A106" s="10">
         <v>42156</v>
       </c>
       <c r="B106">
@@ -1575,7 +1572,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="11">
+      <c r="A107" s="10">
         <v>42186</v>
       </c>
       <c r="B107">
@@ -1583,7 +1580,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="11">
+      <c r="A108" s="10">
         <v>42217</v>
       </c>
       <c r="B108">
@@ -1591,7 +1588,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="11">
+      <c r="A109" s="10">
         <v>42248</v>
       </c>
       <c r="B109">
@@ -1599,7 +1596,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="11">
+      <c r="A110" s="10">
         <v>42278</v>
       </c>
       <c r="B110">
@@ -1607,7 +1604,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="11">
+      <c r="A111" s="10">
         <v>42309</v>
       </c>
       <c r="B111">
@@ -1615,7 +1612,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="11">
+      <c r="A112" s="10">
         <v>42339</v>
       </c>
       <c r="B112">
@@ -1623,7 +1620,7 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="11">
+      <c r="A113" s="10">
         <v>42370</v>
       </c>
       <c r="B113">
@@ -1631,7 +1628,7 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="11">
+      <c r="A114" s="10">
         <v>42401</v>
       </c>
       <c r="B114">
@@ -1639,7 +1636,7 @@
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="11">
+      <c r="A115" s="10">
         <v>42430</v>
       </c>
       <c r="B115">
@@ -1647,7 +1644,7 @@
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="11">
+      <c r="A116" s="10">
         <v>42461</v>
       </c>
       <c r="B116">
@@ -1655,7 +1652,7 @@
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="11">
+      <c r="A117" s="10">
         <v>42491</v>
       </c>
       <c r="B117">
@@ -1663,7 +1660,7 @@
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="11">
+      <c r="A118" s="10">
         <v>42522</v>
       </c>
       <c r="B118">
@@ -1671,7 +1668,7 @@
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="11">
+      <c r="A119" s="10">
         <v>42552</v>
       </c>
       <c r="B119">
@@ -1679,7 +1676,7 @@
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="11">
+      <c r="A120" s="10">
         <v>42583</v>
       </c>
       <c r="B120">
@@ -1687,7 +1684,7 @@
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="11">
+      <c r="A121" s="10">
         <v>42614</v>
       </c>
       <c r="B121">
@@ -1695,7 +1692,7 @@
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="11">
+      <c r="A122" s="10">
         <v>42644</v>
       </c>
       <c r="B122">
@@ -1703,7 +1700,7 @@
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="11">
+      <c r="A123" s="10">
         <v>42675</v>
       </c>
       <c r="B123">
@@ -1711,7 +1708,7 @@
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="11">
+      <c r="A124" s="10">
         <v>42705</v>
       </c>
       <c r="B124">
@@ -1719,7 +1716,7 @@
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="11">
+      <c r="A125" s="10">
         <v>42736</v>
       </c>
       <c r="B125">
@@ -1727,7 +1724,7 @@
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="11">
+      <c r="A126" s="10">
         <v>42767</v>
       </c>
       <c r="B126">
@@ -1735,7 +1732,7 @@
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="11">
+      <c r="A127" s="10">
         <v>42795</v>
       </c>
       <c r="B127">
@@ -1743,7 +1740,7 @@
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="11">
+      <c r="A128" s="10">
         <v>42826</v>
       </c>
       <c r="B128">
@@ -1751,7 +1748,7 @@
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="11">
+      <c r="A129" s="10">
         <v>42856</v>
       </c>
       <c r="B129">
@@ -1759,7 +1756,7 @@
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="11">
+      <c r="A130" s="10">
         <v>42887</v>
       </c>
       <c r="B130">
@@ -1767,7 +1764,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="11">
+      <c r="A131" s="10">
         <v>42917</v>
       </c>
       <c r="B131">
@@ -1775,7 +1772,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="11">
+      <c r="A132" s="10">
         <v>42948</v>
       </c>
       <c r="B132">
@@ -1783,19 +1780,19 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="11"/>
+      <c r="A133" s="10"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="11"/>
+      <c r="A134" s="10"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="11"/>
+      <c r="A135" s="10"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="11"/>
+      <c r="A136" s="10"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="11"/>
+      <c r="A137" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,7 +1804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1823,27 +1820,27 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1852,7 +1849,7 @@
       <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>102000</v>
       </c>
     </row>
@@ -1863,7 +1860,7 @@
       <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>3412</v>
       </c>
     </row>
@@ -1874,21 +1871,21 @@
       <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>135000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Progress on Benchmarking Utility Module.
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -142,9 +142,6 @@
     <t>PAFA</t>
   </si>
   <si>
-    <t>Base-65 Degree Days by Site</t>
-  </si>
-  <si>
     <t>The last 36 months are accurate (Sep-2014 - Aug-2017)</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>btu_per_unit</t>
+  </si>
+  <si>
+    <t>Base-65 Degree Days by Site.  These are Calendar (not fiscal ) Months</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,19 +698,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6">
         <v>1990</v>
@@ -731,20 +731,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1838,7 +1836,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="8"/>
     </row>

</xml_diff>

<commit_message>
More utility functions and finished Page 3 Example.
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26760" windowHeight="11070" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26760" windowHeight="11070"/>
   </bookViews>
   <sheets>
     <sheet name="Building" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="313">
   <si>
     <t>Site ID</t>
   </si>
@@ -61,9 +61,6 @@
     <t>ANSBG1</t>
   </si>
   <si>
-    <t>Animal Control</t>
-  </si>
-  <si>
     <t>2408 Davis Road</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>kWh</t>
   </si>
   <si>
-    <t>Fuel Oil</t>
-  </si>
-  <si>
     <t>Gallons</t>
   </si>
   <si>
@@ -145,22 +139,832 @@
     <t>The last 36 months are accurate (Sep-2014 - Aug-2017)</t>
   </si>
   <si>
-    <t>BIGDIP</t>
-  </si>
-  <si>
-    <t>1920 Lathrop Street</t>
-  </si>
-  <si>
-    <t>Big Dipper Ice Arena</t>
-  </si>
-  <si>
-    <t>Ice Arena</t>
-  </si>
-  <si>
     <t>btu_per_unit</t>
   </si>
   <si>
     <t>Base-65 Degree Days by Site.  These are Calendar (not fiscal ) Months</t>
+  </si>
+  <si>
+    <t>Oil #1</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>MMBtu</t>
+  </si>
+  <si>
+    <t>klbs</t>
+  </si>
+  <si>
+    <t>lbs</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>SD-Denali Elementary</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>SD-Nordale Elementary</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>SD-Lathrop High</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>SD-Hunter Elementary</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>SD-University Park Elementary</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>SD-Barnette Magnet</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>SD-Joy Elementary</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>SD-Salcha Elementary</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>SD-Nutrition Services Center</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>SD-Admin Center</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>SD-North Pole Elementary</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>SD-Ryan Middle</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>SD-Hutchison High</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>SD-Facilities Management</t>
+  </si>
+  <si>
+    <t>15A</t>
+  </si>
+  <si>
+    <t>SD-Krize Building</t>
+  </si>
+  <si>
+    <t>15B</t>
+  </si>
+  <si>
+    <t>SD-Grounds</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>SD-Anderson Elementary</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>SD-Ben Eielson JR/SR</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>SD-North Pole Middle</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>SD-North Pole High</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>SD-Tanana Middle</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>SD-West Valley High</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>SD-Woodriver Elementary</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>SD-Badger Elementary</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>SD-Pearl Creek Elementary</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>SD-Two Rivers Elementary</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>SD-Weller Elementary</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>SD-Ticasuk Brown Elementary</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>SD-Effie Kokrine Charter (HlA)</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>SD-Ladd Elementary</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>SD-Arctic Light Elementary</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>SD-Anne Wien Elementary</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>SD-Chinook Charter</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>SD-Crawford Elementary</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>SD-Randy Smith Middle</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>SD-Star of the North Charter</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>SD-Watershed Charter</t>
+  </si>
+  <si>
+    <t>ADLER</t>
+  </si>
+  <si>
+    <t>FNSB-Adler School building</t>
+  </si>
+  <si>
+    <t>FNSB-Animal Control</t>
+  </si>
+  <si>
+    <t>ASLC18</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Palace Saloon C18</t>
+  </si>
+  <si>
+    <t>ASLC21</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk South Seasonal Water</t>
+  </si>
+  <si>
+    <t>ASLC47</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Barn Cabin 47</t>
+  </si>
+  <si>
+    <t>ASLC52</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Cabin 52/Guard Shack</t>
+  </si>
+  <si>
+    <t>ASLCHU</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk - Office (Cab 19)</t>
+  </si>
+  <si>
+    <t>ASLCV1</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Civic Center</t>
+  </si>
+  <si>
+    <t>ASLELC1</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk East Electrical Serv</t>
+  </si>
+  <si>
+    <t>ASLELC2</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk West Electrical Serv</t>
+  </si>
+  <si>
+    <t>ASLGDM</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Gold Dome</t>
+  </si>
+  <si>
+    <t>ASLGP2</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk East Parking Lot</t>
+  </si>
+  <si>
+    <t>ASLHIS</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Historical Society</t>
+  </si>
+  <si>
+    <t>ASLPIH</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Pioneer Hall</t>
+  </si>
+  <si>
+    <t>ASLPL1</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk West Parkng Lot/Sign</t>
+  </si>
+  <si>
+    <t>ASLSEA</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk North Seasonal Water</t>
+  </si>
+  <si>
+    <t>ASLSQD</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Square Dance Hall</t>
+  </si>
+  <si>
+    <t>ASLTVR</t>
+  </si>
+  <si>
+    <t>FNSB-Pioneer Pk Railroad Museum</t>
+  </si>
+  <si>
+    <t>BALHHW</t>
+  </si>
+  <si>
+    <t>FNSB-Solid Waste Baler/Office/HHW</t>
+  </si>
+  <si>
+    <t>BAOBG1</t>
+  </si>
+  <si>
+    <t>FNSB-JHAC</t>
+  </si>
+  <si>
+    <t>BAP001</t>
+  </si>
+  <si>
+    <t>FNSB-Bernice Aldridge Park</t>
+  </si>
+  <si>
+    <t>BENBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Solid Waste Entrance Scales</t>
+  </si>
+  <si>
+    <t>BHPBHG</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Garage</t>
+  </si>
+  <si>
+    <t>BHPBHL</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Timing Building</t>
+  </si>
+  <si>
+    <t>BHPBHW</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Warm-up Building</t>
+  </si>
+  <si>
+    <t>BHPCCS</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Ski Building</t>
+  </si>
+  <si>
+    <t>BHPSKI1</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Ski Trail #1</t>
+  </si>
+  <si>
+    <t>BHPSKI2</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Ski Trail #2</t>
+  </si>
+  <si>
+    <t>BHPSKI3</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Ski Trail #3</t>
+  </si>
+  <si>
+    <t>BHPSKI4</t>
+  </si>
+  <si>
+    <t>FNSB-Birch Hill Ski Trail #4</t>
+  </si>
+  <si>
+    <t>CACBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Carlson Center</t>
+  </si>
+  <si>
+    <t>CBS001</t>
+  </si>
+  <si>
+    <t>FNSB-Centennial Bridge South</t>
+  </si>
+  <si>
+    <t>CEC</t>
+  </si>
+  <si>
+    <t>SD-CEC-Star Charter</t>
+  </si>
+  <si>
+    <t>CLX001</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Chena Lakes Rec Area</t>
+  </si>
+  <si>
+    <t>CLX002</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Chena Lakes Rec Park</t>
+  </si>
+  <si>
+    <t>CLX003</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Chena River Lakes Rec Proj</t>
+  </si>
+  <si>
+    <t>CLX004</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Chena River Lakes Proj A</t>
+  </si>
+  <si>
+    <t>CLXES1</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Entrance Station</t>
+  </si>
+  <si>
+    <t>CLXGP2</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA River Park General Area</t>
+  </si>
+  <si>
+    <t>CLXSM1</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Maintenance Bunker</t>
+  </si>
+  <si>
+    <t>CLXSO1</t>
+  </si>
+  <si>
+    <t>FNSB-CLRA Office/Shop</t>
+  </si>
+  <si>
+    <t>CRB001</t>
+  </si>
+  <si>
+    <t>FNSB-Chena River Bridge</t>
+  </si>
+  <si>
+    <t>CSP001</t>
+  </si>
+  <si>
+    <t>FNSB-Crosson Street Park</t>
+  </si>
+  <si>
+    <t>DIPMP1</t>
+  </si>
+  <si>
+    <t>FNSB-Big Dipper</t>
+  </si>
+  <si>
+    <t>DOGPRK</t>
+  </si>
+  <si>
+    <t>FNSB-South Davis Dog Park Lighting</t>
+  </si>
+  <si>
+    <t>Emer S T</t>
+  </si>
+  <si>
+    <t>SD-FNSB Emergency Service Tower</t>
+  </si>
+  <si>
+    <t>GF001</t>
+  </si>
+  <si>
+    <t>FNSB-Gillam Field</t>
+  </si>
+  <si>
+    <t>GFP001</t>
+  </si>
+  <si>
+    <t>FNSB-Griffin Park</t>
+  </si>
+  <si>
+    <t>GRP001</t>
+  </si>
+  <si>
+    <t>FNSB-Growden Park</t>
+  </si>
+  <si>
+    <t>GRPLFT</t>
+  </si>
+  <si>
+    <t>FNSB-Growden Park Lift Station</t>
+  </si>
+  <si>
+    <t>GSWNP</t>
+  </si>
+  <si>
+    <t>FNSB-General Serv Wareh North Pole</t>
+  </si>
+  <si>
+    <t>HEMBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Solid Waste Heavy Equip Bldg</t>
+  </si>
+  <si>
+    <t>HEZ001</t>
+  </si>
+  <si>
+    <t>FNSB-Hez Ray Sport Complex</t>
+  </si>
+  <si>
+    <t>HSPSWP</t>
+  </si>
+  <si>
+    <t>FNSB-Hamme Swimming Pool</t>
+  </si>
+  <si>
+    <t>KEP001</t>
+  </si>
+  <si>
+    <t>FNSB-Kendall Park</t>
+  </si>
+  <si>
+    <t>KIP001</t>
+  </si>
+  <si>
+    <t>FNSB-Kiana Park</t>
+  </si>
+  <si>
+    <t>KWP001</t>
+  </si>
+  <si>
+    <t>FNSB-Kiwanis Park</t>
+  </si>
+  <si>
+    <t>LEABG1</t>
+  </si>
+  <si>
+    <t>FNSB-Solid Waste Leachate Building</t>
+  </si>
+  <si>
+    <t>LF001</t>
+  </si>
+  <si>
+    <t>FNSB-Lions Field</t>
+  </si>
+  <si>
+    <t>MF001</t>
+  </si>
+  <si>
+    <t>FNSB-Marlin Field</t>
+  </si>
+  <si>
+    <t>MNPPRK</t>
+  </si>
+  <si>
+    <t>FNSB-Morning Star Park</t>
+  </si>
+  <si>
+    <t>MSLL001</t>
+  </si>
+  <si>
+    <t>FNSB-Moore Street Little League</t>
+  </si>
+  <si>
+    <t>MSP001</t>
+  </si>
+  <si>
+    <t>FNSB-Midnight Sun Lions Park</t>
+  </si>
+  <si>
+    <t>MSRSWP</t>
+  </si>
+  <si>
+    <t>FNSB-Mary Siah Rec Center</t>
+  </si>
+  <si>
+    <t>MSWBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Marika St Maintenance Shop</t>
+  </si>
+  <si>
+    <t>MSWBG2</t>
+  </si>
+  <si>
+    <t>FNSB-Marika St Maintenance Storage</t>
+  </si>
+  <si>
+    <t>MSWWAR</t>
+  </si>
+  <si>
+    <t>FNSB-Marika St Warehouse-Gen Svcs</t>
+  </si>
+  <si>
+    <t>MTP001</t>
+  </si>
+  <si>
+    <t>FNSB-Mertyle Thomas Park</t>
+  </si>
+  <si>
+    <t>NBP001</t>
+  </si>
+  <si>
+    <t>FNSB-Nussbaumer Park</t>
+  </si>
+  <si>
+    <t>NPL</t>
+  </si>
+  <si>
+    <t>FNSB-North Pole Library</t>
+  </si>
+  <si>
+    <t>NPP001</t>
+  </si>
+  <si>
+    <t>FNSB-North Pole Park</t>
+  </si>
+  <si>
+    <t>NRP001</t>
+  </si>
+  <si>
+    <t>FNSB-Newby Road Park</t>
+  </si>
+  <si>
+    <t>NWLBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Noel Wien Library</t>
+  </si>
+  <si>
+    <t>NWLP01</t>
+  </si>
+  <si>
+    <t>FNSB-Noel Wein Library Park</t>
+  </si>
+  <si>
+    <t>NWP001</t>
+  </si>
+  <si>
+    <t>FNSB-Newby Park</t>
+  </si>
+  <si>
+    <t>PRW</t>
+  </si>
+  <si>
+    <t>FNSB-Peger Road West - Trans Garag</t>
+  </si>
+  <si>
+    <t>SF001</t>
+  </si>
+  <si>
+    <t>FNSB-Stockton Field</t>
+  </si>
+  <si>
+    <t>SHW001</t>
+  </si>
+  <si>
+    <t>FNSB-Shoreway Pk-Downtown Walk Brdg</t>
+  </si>
+  <si>
+    <t>STRBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Solid Waste Storage Shed</t>
+  </si>
+  <si>
+    <t>TRANS01</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Farmers Loop Rd West</t>
+  </si>
+  <si>
+    <t>TRANS02</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Midway</t>
+  </si>
+  <si>
+    <t>TRANS03</t>
+  </si>
+  <si>
+    <t>FNSB-TS - 35 Mi Richardson Hwy</t>
+  </si>
+  <si>
+    <t>TRANS04</t>
+  </si>
+  <si>
+    <t>FNSB-TS - 18 Mi CHSR - Two Rivers</t>
+  </si>
+  <si>
+    <t>TRANS05</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Fox Dumpster Site</t>
+  </si>
+  <si>
+    <t>TRANS06</t>
+  </si>
+  <si>
+    <t>FNSB-TS - North Pole</t>
+  </si>
+  <si>
+    <t>TRANS07</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Old Chena Ridge Rd</t>
+  </si>
+  <si>
+    <t>TRANS08</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Farmers Loop Rd East</t>
+  </si>
+  <si>
+    <t>TRANS09</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Badger and Holmes Rd</t>
+  </si>
+  <si>
+    <t>TRANS10</t>
+  </si>
+  <si>
+    <t>FNSB-TS - Little Shot Rd Ester</t>
+  </si>
+  <si>
+    <t>TRGR</t>
+  </si>
+  <si>
+    <t>FNSB-Transit Garage</t>
+  </si>
+  <si>
+    <t>TRPAIR</t>
+  </si>
+  <si>
+    <t>FNSB-Transit Park/Air Qual Trailer</t>
+  </si>
+  <si>
+    <t>TRPBG1</t>
+  </si>
+  <si>
+    <t>FNSB-Transit Park/Downtown Terminal</t>
+  </si>
+  <si>
+    <t>TRS001</t>
+  </si>
+  <si>
+    <t>FNSB-Two Rivers Sports Complex</t>
+  </si>
+  <si>
+    <t>VMP001</t>
+  </si>
+  <si>
+    <t>FNSB-Veterans Memorial Park</t>
+  </si>
+  <si>
+    <t>WF001</t>
+  </si>
+  <si>
+    <t>FNSB-Weeks Field</t>
+  </si>
+  <si>
+    <t>WSPGAR</t>
+  </si>
+  <si>
+    <t>FNSB-Wescott Garage / Zamboni Rm</t>
+  </si>
+  <si>
+    <t>WSPP01</t>
+  </si>
+  <si>
+    <t>FNSB-Wendal Street Pedestrian Path</t>
+  </si>
+  <si>
+    <t>WSPSWP</t>
+  </si>
+  <si>
+    <t>FNSB-Wescott Swimming Pool</t>
   </si>
 </sst>
 </file>
@@ -251,7 +1055,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -273,6 +1077,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -588,21 +1393,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="24" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -642,88 +1447,1941 @@
     </row>
     <row r="4" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>1993</v>
-      </c>
-      <c r="G5" s="2">
-        <v>14000</v>
+        <v>45</v>
+      </c>
+      <c r="G5" s="11">
+        <v>10123</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="G25" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G30" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>98</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" t="s">
+        <v>103</v>
+      </c>
+      <c r="G34" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G35" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+      <c r="G36" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="G37" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="G39" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="G40" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G41" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
         <v>13</v>
       </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6">
-        <v>1990</v>
-      </c>
-      <c r="G6" s="2">
-        <v>23000</v>
-      </c>
-      <c r="I6" t="s">
-        <v>37</v>
+      <c r="F43">
+        <v>1993</v>
+      </c>
+      <c r="G43" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" t="s">
+        <v>122</v>
+      </c>
+      <c r="G44" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" t="s">
+        <v>126</v>
+      </c>
+      <c r="G46" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="G47" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="G48" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>131</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="G49" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" t="s">
+        <v>134</v>
+      </c>
+      <c r="G50" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" t="s">
+        <v>136</v>
+      </c>
+      <c r="G51" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>137</v>
+      </c>
+      <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="G53" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>143</v>
+      </c>
+      <c r="B55" t="s">
+        <v>144</v>
+      </c>
+      <c r="G55" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="G56" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>147</v>
+      </c>
+      <c r="B57" t="s">
+        <v>148</v>
+      </c>
+      <c r="G57" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="B58" t="s">
+        <v>150</v>
+      </c>
+      <c r="G58" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" t="s">
+        <v>152</v>
+      </c>
+      <c r="G59" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" t="s">
+        <v>154</v>
+      </c>
+      <c r="G60" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" t="s">
+        <v>156</v>
+      </c>
+      <c r="G61" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" t="s">
+        <v>158</v>
+      </c>
+      <c r="G62" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>159</v>
+      </c>
+      <c r="B63" t="s">
+        <v>160</v>
+      </c>
+      <c r="G63" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>161</v>
+      </c>
+      <c r="B64" t="s">
+        <v>162</v>
+      </c>
+      <c r="G64" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" t="s">
+        <v>164</v>
+      </c>
+      <c r="G65" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" t="s">
+        <v>168</v>
+      </c>
+      <c r="G67" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" t="s">
+        <v>170</v>
+      </c>
+      <c r="G68" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" t="s">
+        <v>172</v>
+      </c>
+      <c r="G69" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" t="s">
+        <v>174</v>
+      </c>
+      <c r="G70" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>175</v>
+      </c>
+      <c r="B71" t="s">
+        <v>176</v>
+      </c>
+      <c r="G71" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72" t="s">
+        <v>178</v>
+      </c>
+      <c r="G72" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" t="s">
+        <v>180</v>
+      </c>
+      <c r="G73" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>181</v>
+      </c>
+      <c r="B74" t="s">
+        <v>182</v>
+      </c>
+      <c r="G74" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" t="s">
+        <v>184</v>
+      </c>
+      <c r="G75" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>185</v>
+      </c>
+      <c r="B76" t="s">
+        <v>186</v>
+      </c>
+      <c r="G76" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>187</v>
+      </c>
+      <c r="B77" t="s">
+        <v>188</v>
+      </c>
+      <c r="G77" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>189</v>
+      </c>
+      <c r="B78" t="s">
+        <v>190</v>
+      </c>
+      <c r="G78" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>191</v>
+      </c>
+      <c r="B79" t="s">
+        <v>192</v>
+      </c>
+      <c r="G79" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>193</v>
+      </c>
+      <c r="B80" t="s">
+        <v>194</v>
+      </c>
+      <c r="G80" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>195</v>
+      </c>
+      <c r="B81" t="s">
+        <v>196</v>
+      </c>
+      <c r="G81" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I81" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>197</v>
+      </c>
+      <c r="B82" t="s">
+        <v>198</v>
+      </c>
+      <c r="G82" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>199</v>
+      </c>
+      <c r="B83" t="s">
+        <v>200</v>
+      </c>
+      <c r="G83" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I83" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>201</v>
+      </c>
+      <c r="B84" t="s">
+        <v>202</v>
+      </c>
+      <c r="G84" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>203</v>
+      </c>
+      <c r="B85" t="s">
+        <v>204</v>
+      </c>
+      <c r="G85" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>205</v>
+      </c>
+      <c r="B86" t="s">
+        <v>206</v>
+      </c>
+      <c r="G86" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>207</v>
+      </c>
+      <c r="B87" t="s">
+        <v>208</v>
+      </c>
+      <c r="G87" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I87" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>209</v>
+      </c>
+      <c r="B88" t="s">
+        <v>210</v>
+      </c>
+      <c r="G88" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I88" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>211</v>
+      </c>
+      <c r="B89" t="s">
+        <v>212</v>
+      </c>
+      <c r="G89" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I89" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>213</v>
+      </c>
+      <c r="B90" t="s">
+        <v>214</v>
+      </c>
+      <c r="G90" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I90" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>215</v>
+      </c>
+      <c r="B91" t="s">
+        <v>216</v>
+      </c>
+      <c r="G91" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I91" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>217</v>
+      </c>
+      <c r="B92" t="s">
+        <v>218</v>
+      </c>
+      <c r="G92" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I92" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>219</v>
+      </c>
+      <c r="B93" t="s">
+        <v>220</v>
+      </c>
+      <c r="G93" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I93" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>221</v>
+      </c>
+      <c r="B94" t="s">
+        <v>222</v>
+      </c>
+      <c r="G94" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I94" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>223</v>
+      </c>
+      <c r="B95" t="s">
+        <v>224</v>
+      </c>
+      <c r="G95" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I95" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96" t="s">
+        <v>226</v>
+      </c>
+      <c r="G96" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I96" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>227</v>
+      </c>
+      <c r="B97" t="s">
+        <v>228</v>
+      </c>
+      <c r="G97" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>229</v>
+      </c>
+      <c r="B98" t="s">
+        <v>230</v>
+      </c>
+      <c r="G98" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>231</v>
+      </c>
+      <c r="B99" t="s">
+        <v>232</v>
+      </c>
+      <c r="G99" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I99" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>233</v>
+      </c>
+      <c r="B100" t="s">
+        <v>234</v>
+      </c>
+      <c r="G100" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I100" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>235</v>
+      </c>
+      <c r="B101" t="s">
+        <v>236</v>
+      </c>
+      <c r="G101" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I101" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>237</v>
+      </c>
+      <c r="B102" t="s">
+        <v>238</v>
+      </c>
+      <c r="G102" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I102" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>239</v>
+      </c>
+      <c r="B103" t="s">
+        <v>240</v>
+      </c>
+      <c r="G103" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I103" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>241</v>
+      </c>
+      <c r="B104" t="s">
+        <v>242</v>
+      </c>
+      <c r="G104" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I104" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>243</v>
+      </c>
+      <c r="B105" t="s">
+        <v>244</v>
+      </c>
+      <c r="G105" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>245</v>
+      </c>
+      <c r="B106" t="s">
+        <v>246</v>
+      </c>
+      <c r="G106" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I106" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>247</v>
+      </c>
+      <c r="B107" t="s">
+        <v>248</v>
+      </c>
+      <c r="G107" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I107" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>249</v>
+      </c>
+      <c r="B108" t="s">
+        <v>250</v>
+      </c>
+      <c r="G108" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>251</v>
+      </c>
+      <c r="B109" t="s">
+        <v>252</v>
+      </c>
+      <c r="G109" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I109" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>253</v>
+      </c>
+      <c r="B110" t="s">
+        <v>254</v>
+      </c>
+      <c r="G110" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I110" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>255</v>
+      </c>
+      <c r="B111" t="s">
+        <v>256</v>
+      </c>
+      <c r="G111" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>257</v>
+      </c>
+      <c r="B112" t="s">
+        <v>258</v>
+      </c>
+      <c r="G112" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>259</v>
+      </c>
+      <c r="B113" t="s">
+        <v>260</v>
+      </c>
+      <c r="G113" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I113" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>261</v>
+      </c>
+      <c r="B114" t="s">
+        <v>262</v>
+      </c>
+      <c r="G114" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I114" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>263</v>
+      </c>
+      <c r="B115" t="s">
+        <v>264</v>
+      </c>
+      <c r="G115" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I115" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>265</v>
+      </c>
+      <c r="B116" t="s">
+        <v>266</v>
+      </c>
+      <c r="G116" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I116" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>267</v>
+      </c>
+      <c r="B117" t="s">
+        <v>268</v>
+      </c>
+      <c r="G117" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I117" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>269</v>
+      </c>
+      <c r="B118" t="s">
+        <v>270</v>
+      </c>
+      <c r="G118" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I118" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>271</v>
+      </c>
+      <c r="B119" t="s">
+        <v>272</v>
+      </c>
+      <c r="G119" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I119" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>273</v>
+      </c>
+      <c r="B120" t="s">
+        <v>274</v>
+      </c>
+      <c r="G120" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I120" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>275</v>
+      </c>
+      <c r="B121" t="s">
+        <v>276</v>
+      </c>
+      <c r="G121" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>277</v>
+      </c>
+      <c r="B122" t="s">
+        <v>278</v>
+      </c>
+      <c r="G122" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I122" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>279</v>
+      </c>
+      <c r="B123" t="s">
+        <v>280</v>
+      </c>
+      <c r="G123" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I123" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>281</v>
+      </c>
+      <c r="B124" t="s">
+        <v>282</v>
+      </c>
+      <c r="G124" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I124" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>283</v>
+      </c>
+      <c r="B125" t="s">
+        <v>284</v>
+      </c>
+      <c r="G125" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I125" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>285</v>
+      </c>
+      <c r="B126" t="s">
+        <v>286</v>
+      </c>
+      <c r="G126" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I126" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>287</v>
+      </c>
+      <c r="B127" t="s">
+        <v>288</v>
+      </c>
+      <c r="G127" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I127" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>289</v>
+      </c>
+      <c r="B128" t="s">
+        <v>290</v>
+      </c>
+      <c r="G128" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I128" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>291</v>
+      </c>
+      <c r="B129" t="s">
+        <v>292</v>
+      </c>
+      <c r="G129" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I129" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>293</v>
+      </c>
+      <c r="B130" t="s">
+        <v>294</v>
+      </c>
+      <c r="G130" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I130" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>295</v>
+      </c>
+      <c r="B131" t="s">
+        <v>296</v>
+      </c>
+      <c r="G131" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I131" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>297</v>
+      </c>
+      <c r="B132" t="s">
+        <v>298</v>
+      </c>
+      <c r="G132" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I132" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>299</v>
+      </c>
+      <c r="B133" t="s">
+        <v>300</v>
+      </c>
+      <c r="G133" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I133" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>301</v>
+      </c>
+      <c r="B134" t="s">
+        <v>302</v>
+      </c>
+      <c r="G134" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I134" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>303</v>
+      </c>
+      <c r="B135" t="s">
+        <v>304</v>
+      </c>
+      <c r="G135" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I135" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>305</v>
+      </c>
+      <c r="B136" t="s">
+        <v>306</v>
+      </c>
+      <c r="G136" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I136" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>307</v>
+      </c>
+      <c r="B137" t="s">
+        <v>308</v>
+      </c>
+      <c r="G137" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I137" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>309</v>
+      </c>
+      <c r="B138" t="s">
+        <v>310</v>
+      </c>
+      <c r="G138" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I138" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>311</v>
+      </c>
+      <c r="B139" t="s">
+        <v>312</v>
+      </c>
+      <c r="G139" s="11">
+        <v>10123</v>
+      </c>
+      <c r="I139" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A21" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -731,7 +3389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
@@ -739,20 +3397,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1805,7 +4463,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1816,38 +4474,38 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
         <v>30</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
       </c>
       <c r="C5" s="2">
         <v>102000</v>
@@ -1855,10 +4513,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" t="s">
-        <v>33</v>
       </c>
       <c r="C6" s="2">
         <v>3412</v>
@@ -1866,23 +4524,47 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2">
         <v>135000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1000000</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1194000</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1194</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>

</xml_diff>

<commit_message>
Added Site Category to Building Info Spreadsheet.
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="317">
   <si>
     <t>Site ID</t>
   </si>
@@ -965,6 +965,18 @@
   </si>
   <si>
     <t>FNSB-Wescott Swimming Pool</t>
+  </si>
+  <si>
+    <t>Site Category</t>
+  </si>
+  <si>
+    <t>site_category</t>
+  </si>
+  <si>
+    <t>School District</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -1393,30 +1405,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K139"/>
+  <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1424,28 +1437,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
@@ -1453,561 +1469,678 @@
         <v>15</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H5" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>315</v>
+      </c>
+      <c r="H6" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>315</v>
+      </c>
+      <c r="H7" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>315</v>
+      </c>
+      <c r="H8" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>315</v>
+      </c>
+      <c r="H9" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>315</v>
+      </c>
+      <c r="H10" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>315</v>
+      </c>
+      <c r="H11" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>315</v>
+      </c>
+      <c r="H12" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>315</v>
+      </c>
+      <c r="H13" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>315</v>
+      </c>
+      <c r="H14" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>64</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>315</v>
+      </c>
+      <c r="H15" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>315</v>
+      </c>
+      <c r="H16" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>68</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>315</v>
+      </c>
+      <c r="H17" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>70</v>
       </c>
       <c r="B18" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>315</v>
+      </c>
+      <c r="H18" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
       <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>315</v>
+      </c>
+      <c r="H19" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>74</v>
       </c>
       <c r="B20" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>315</v>
+      </c>
+      <c r="H20" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
       <c r="B21" t="s">
         <v>77</v>
       </c>
-      <c r="G21" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>315</v>
+      </c>
+      <c r="H21" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>78</v>
       </c>
       <c r="B22" t="s">
         <v>79</v>
       </c>
-      <c r="G22" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>315</v>
+      </c>
+      <c r="H22" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
       <c r="B23" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>315</v>
+      </c>
+      <c r="H23" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
       <c r="B24" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>315</v>
+      </c>
+      <c r="H24" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>84</v>
       </c>
       <c r="B25" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>315</v>
+      </c>
+      <c r="H25" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>86</v>
       </c>
       <c r="B26" t="s">
         <v>87</v>
       </c>
-      <c r="G26" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>315</v>
+      </c>
+      <c r="H26" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>88</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>315</v>
+      </c>
+      <c r="H27" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>90</v>
       </c>
       <c r="B28" t="s">
         <v>91</v>
       </c>
-      <c r="G28" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>315</v>
+      </c>
+      <c r="H28" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>92</v>
       </c>
       <c r="B29" t="s">
         <v>93</v>
       </c>
-      <c r="G29" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>315</v>
+      </c>
+      <c r="H29" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>94</v>
       </c>
       <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="G30" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>315</v>
+      </c>
+      <c r="H30" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>97</v>
       </c>
-      <c r="G31" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>315</v>
+      </c>
+      <c r="H31" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>98</v>
       </c>
       <c r="B32" t="s">
         <v>99</v>
       </c>
-      <c r="G32" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>315</v>
+      </c>
+      <c r="H32" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>100</v>
       </c>
       <c r="B33" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>315</v>
+      </c>
+      <c r="H33" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>102</v>
       </c>
       <c r="B34" t="s">
         <v>103</v>
       </c>
-      <c r="G34" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>315</v>
+      </c>
+      <c r="H34" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>104</v>
       </c>
       <c r="B35" t="s">
         <v>105</v>
       </c>
-      <c r="G35" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>315</v>
+      </c>
+      <c r="H35" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>106</v>
       </c>
       <c r="B36" t="s">
         <v>107</v>
       </c>
-      <c r="G36" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>315</v>
+      </c>
+      <c r="H36" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>108</v>
       </c>
       <c r="B37" t="s">
         <v>109</v>
       </c>
-      <c r="G37" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>315</v>
+      </c>
+      <c r="H37" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>110</v>
       </c>
       <c r="B38" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>315</v>
+      </c>
+      <c r="H38" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>112</v>
       </c>
       <c r="B39" t="s">
         <v>113</v>
       </c>
-      <c r="G39" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>315</v>
+      </c>
+      <c r="H39" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>114</v>
       </c>
       <c r="B40" t="s">
         <v>115</v>
       </c>
-      <c r="G40" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>315</v>
+      </c>
+      <c r="H40" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>116</v>
       </c>
       <c r="B41" t="s">
         <v>117</v>
       </c>
-      <c r="G41" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I41" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>315</v>
+      </c>
+      <c r="H41" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>118</v>
       </c>
       <c r="B42" t="s">
         <v>119</v>
       </c>
-      <c r="G42" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>316</v>
+      </c>
+      <c r="H42" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -2015,1365 +2148,1656 @@
         <v>120</v>
       </c>
       <c r="C43" t="s">
+        <v>316</v>
+      </c>
+      <c r="D43" t="s">
         <v>11</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>12</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>13</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>1993</v>
       </c>
-      <c r="G43" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H43" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>121</v>
       </c>
       <c r="B44" t="s">
         <v>122</v>
       </c>
-      <c r="G44" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I44" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>316</v>
+      </c>
+      <c r="H44" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>123</v>
       </c>
       <c r="B45" t="s">
         <v>124</v>
       </c>
-      <c r="G45" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>316</v>
+      </c>
+      <c r="H45" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>125</v>
       </c>
       <c r="B46" t="s">
         <v>126</v>
       </c>
-      <c r="G46" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I46" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>316</v>
+      </c>
+      <c r="H46" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>127</v>
       </c>
       <c r="B47" t="s">
         <v>128</v>
       </c>
-      <c r="G47" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I47" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>316</v>
+      </c>
+      <c r="H47" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>129</v>
       </c>
       <c r="B48" t="s">
         <v>130</v>
       </c>
-      <c r="G48" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I48" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>316</v>
+      </c>
+      <c r="H48" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>131</v>
       </c>
       <c r="B49" t="s">
         <v>132</v>
       </c>
-      <c r="G49" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I49" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>316</v>
+      </c>
+      <c r="H49" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>133</v>
       </c>
       <c r="B50" t="s">
         <v>134</v>
       </c>
-      <c r="G50" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>316</v>
+      </c>
+      <c r="H50" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>135</v>
       </c>
       <c r="B51" t="s">
         <v>136</v>
       </c>
-      <c r="G51" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I51" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>316</v>
+      </c>
+      <c r="H51" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>137</v>
       </c>
       <c r="B52" t="s">
         <v>138</v>
       </c>
-      <c r="G52" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I52" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>316</v>
+      </c>
+      <c r="H52" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J52" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>139</v>
       </c>
       <c r="B53" t="s">
         <v>140</v>
       </c>
-      <c r="G53" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I53" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>316</v>
+      </c>
+      <c r="H53" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>141</v>
       </c>
       <c r="B54" t="s">
         <v>142</v>
       </c>
-      <c r="G54" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I54" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>316</v>
+      </c>
+      <c r="H54" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>143</v>
       </c>
       <c r="B55" t="s">
         <v>144</v>
       </c>
-      <c r="G55" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I55" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>316</v>
+      </c>
+      <c r="H55" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J55" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>145</v>
       </c>
       <c r="B56" t="s">
         <v>146</v>
       </c>
-      <c r="G56" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I56" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>316</v>
+      </c>
+      <c r="H56" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J56" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>147</v>
       </c>
       <c r="B57" t="s">
         <v>148</v>
       </c>
-      <c r="G57" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I57" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>316</v>
+      </c>
+      <c r="H57" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>149</v>
       </c>
       <c r="B58" t="s">
         <v>150</v>
       </c>
-      <c r="G58" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I58" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>316</v>
+      </c>
+      <c r="H58" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>151</v>
       </c>
       <c r="B59" t="s">
         <v>152</v>
       </c>
-      <c r="G59" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I59" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>316</v>
+      </c>
+      <c r="H59" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>153</v>
       </c>
       <c r="B60" t="s">
         <v>154</v>
       </c>
-      <c r="G60" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I60" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>316</v>
+      </c>
+      <c r="H60" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>155</v>
       </c>
       <c r="B61" t="s">
         <v>156</v>
       </c>
-      <c r="G61" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I61" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>316</v>
+      </c>
+      <c r="H61" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>157</v>
       </c>
       <c r="B62" t="s">
         <v>158</v>
       </c>
-      <c r="G62" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I62" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>316</v>
+      </c>
+      <c r="H62" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>159</v>
       </c>
       <c r="B63" t="s">
         <v>160</v>
       </c>
-      <c r="G63" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I63" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>316</v>
+      </c>
+      <c r="H63" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J63" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>161</v>
       </c>
       <c r="B64" t="s">
         <v>162</v>
       </c>
-      <c r="G64" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I64" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>316</v>
+      </c>
+      <c r="H64" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J64" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>163</v>
       </c>
       <c r="B65" t="s">
         <v>164</v>
       </c>
-      <c r="G65" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I65" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>316</v>
+      </c>
+      <c r="H65" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>165</v>
       </c>
       <c r="B66" t="s">
         <v>166</v>
       </c>
-      <c r="G66" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I66" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>316</v>
+      </c>
+      <c r="H66" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>167</v>
       </c>
       <c r="B67" t="s">
         <v>168</v>
       </c>
-      <c r="G67" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I67" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>316</v>
+      </c>
+      <c r="H67" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>169</v>
       </c>
       <c r="B68" t="s">
         <v>170</v>
       </c>
-      <c r="G68" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I68" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>316</v>
+      </c>
+      <c r="H68" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>171</v>
       </c>
       <c r="B69" t="s">
         <v>172</v>
       </c>
-      <c r="G69" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I69" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>316</v>
+      </c>
+      <c r="H69" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>173</v>
       </c>
       <c r="B70" t="s">
         <v>174</v>
       </c>
-      <c r="G70" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I70" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>316</v>
+      </c>
+      <c r="H70" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>175</v>
       </c>
       <c r="B71" t="s">
         <v>176</v>
       </c>
-      <c r="G71" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I71" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>316</v>
+      </c>
+      <c r="H71" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>177</v>
       </c>
       <c r="B72" t="s">
         <v>178</v>
       </c>
-      <c r="G72" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I72" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>316</v>
+      </c>
+      <c r="H72" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>179</v>
       </c>
       <c r="B73" t="s">
         <v>180</v>
       </c>
-      <c r="G73" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I73" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>316</v>
+      </c>
+      <c r="H73" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>181</v>
       </c>
       <c r="B74" t="s">
         <v>182</v>
       </c>
-      <c r="G74" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I74" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>316</v>
+      </c>
+      <c r="H74" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>183</v>
       </c>
       <c r="B75" t="s">
         <v>184</v>
       </c>
-      <c r="G75" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I75" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>316</v>
+      </c>
+      <c r="H75" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>185</v>
       </c>
       <c r="B76" t="s">
         <v>186</v>
       </c>
-      <c r="G76" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I76" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>316</v>
+      </c>
+      <c r="H76" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>187</v>
       </c>
       <c r="B77" t="s">
         <v>188</v>
       </c>
-      <c r="G77" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I77" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>316</v>
+      </c>
+      <c r="H77" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>189</v>
       </c>
       <c r="B78" t="s">
         <v>190</v>
       </c>
-      <c r="G78" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I78" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>316</v>
+      </c>
+      <c r="H78" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J78" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>191</v>
       </c>
       <c r="B79" t="s">
         <v>192</v>
       </c>
-      <c r="G79" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I79" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>316</v>
+      </c>
+      <c r="H79" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>193</v>
       </c>
       <c r="B80" t="s">
         <v>194</v>
       </c>
-      <c r="G80" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I80" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>316</v>
+      </c>
+      <c r="H80" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J80" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>195</v>
       </c>
       <c r="B81" t="s">
         <v>196</v>
       </c>
-      <c r="G81" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I81" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>316</v>
+      </c>
+      <c r="H81" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J81" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>197</v>
       </c>
       <c r="B82" t="s">
         <v>198</v>
       </c>
-      <c r="G82" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I82" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>316</v>
+      </c>
+      <c r="H82" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>199</v>
       </c>
       <c r="B83" t="s">
         <v>200</v>
       </c>
-      <c r="G83" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I83" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>316</v>
+      </c>
+      <c r="H83" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J83" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>201</v>
       </c>
       <c r="B84" t="s">
         <v>202</v>
       </c>
-      <c r="G84" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I84" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>316</v>
+      </c>
+      <c r="H84" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>203</v>
       </c>
       <c r="B85" t="s">
         <v>204</v>
       </c>
-      <c r="G85" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I85" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>316</v>
+      </c>
+      <c r="H85" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J85" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>205</v>
       </c>
       <c r="B86" t="s">
         <v>206</v>
       </c>
-      <c r="G86" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I86" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>316</v>
+      </c>
+      <c r="H86" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J86" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>207</v>
       </c>
       <c r="B87" t="s">
         <v>208</v>
       </c>
-      <c r="G87" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I87" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>316</v>
+      </c>
+      <c r="H87" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J87" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>209</v>
       </c>
       <c r="B88" t="s">
         <v>210</v>
       </c>
-      <c r="G88" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I88" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>316</v>
+      </c>
+      <c r="H88" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J88" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>211</v>
       </c>
       <c r="B89" t="s">
         <v>212</v>
       </c>
-      <c r="G89" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I89" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>316</v>
+      </c>
+      <c r="H89" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J89" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>213</v>
       </c>
       <c r="B90" t="s">
         <v>214</v>
       </c>
-      <c r="G90" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I90" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>316</v>
+      </c>
+      <c r="H90" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J90" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>215</v>
       </c>
       <c r="B91" t="s">
         <v>216</v>
       </c>
-      <c r="G91" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I91" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>316</v>
+      </c>
+      <c r="H91" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J91" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>217</v>
       </c>
       <c r="B92" t="s">
         <v>218</v>
       </c>
-      <c r="G92" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I92" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>316</v>
+      </c>
+      <c r="H92" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J92" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>219</v>
       </c>
       <c r="B93" t="s">
         <v>220</v>
       </c>
-      <c r="G93" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I93" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>316</v>
+      </c>
+      <c r="H93" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J93" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>221</v>
       </c>
       <c r="B94" t="s">
         <v>222</v>
       </c>
-      <c r="G94" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I94" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>316</v>
+      </c>
+      <c r="H94" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J94" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>223</v>
       </c>
       <c r="B95" t="s">
         <v>224</v>
       </c>
-      <c r="G95" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I95" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>316</v>
+      </c>
+      <c r="H95" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J95" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>225</v>
       </c>
       <c r="B96" t="s">
         <v>226</v>
       </c>
-      <c r="G96" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I96" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>316</v>
+      </c>
+      <c r="H96" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J96" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>227</v>
       </c>
       <c r="B97" t="s">
         <v>228</v>
       </c>
-      <c r="G97" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I97" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>316</v>
+      </c>
+      <c r="H97" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J97" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>229</v>
       </c>
       <c r="B98" t="s">
         <v>230</v>
       </c>
-      <c r="G98" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I98" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>316</v>
+      </c>
+      <c r="H98" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J98" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>231</v>
       </c>
       <c r="B99" t="s">
         <v>232</v>
       </c>
-      <c r="G99" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I99" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>316</v>
+      </c>
+      <c r="H99" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J99" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>233</v>
       </c>
       <c r="B100" t="s">
         <v>234</v>
       </c>
-      <c r="G100" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I100" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>316</v>
+      </c>
+      <c r="H100" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J100" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>235</v>
       </c>
       <c r="B101" t="s">
         <v>236</v>
       </c>
-      <c r="G101" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I101" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>316</v>
+      </c>
+      <c r="H101" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J101" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>237</v>
       </c>
       <c r="B102" t="s">
         <v>238</v>
       </c>
-      <c r="G102" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I102" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>316</v>
+      </c>
+      <c r="H102" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J102" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>239</v>
       </c>
       <c r="B103" t="s">
         <v>240</v>
       </c>
-      <c r="G103" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I103" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>316</v>
+      </c>
+      <c r="H103" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J103" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>241</v>
       </c>
       <c r="B104" t="s">
         <v>242</v>
       </c>
-      <c r="G104" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I104" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>316</v>
+      </c>
+      <c r="H104" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J104" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>243</v>
       </c>
       <c r="B105" t="s">
         <v>244</v>
       </c>
-      <c r="G105" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I105" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>316</v>
+      </c>
+      <c r="H105" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J105" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>245</v>
       </c>
       <c r="B106" t="s">
         <v>246</v>
       </c>
-      <c r="G106" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I106" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>316</v>
+      </c>
+      <c r="H106" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J106" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>247</v>
       </c>
       <c r="B107" t="s">
         <v>248</v>
       </c>
-      <c r="G107" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I107" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>316</v>
+      </c>
+      <c r="H107" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J107" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>249</v>
       </c>
       <c r="B108" t="s">
         <v>250</v>
       </c>
-      <c r="G108" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I108" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>316</v>
+      </c>
+      <c r="H108" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J108" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>251</v>
       </c>
       <c r="B109" t="s">
         <v>252</v>
       </c>
-      <c r="G109" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I109" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>316</v>
+      </c>
+      <c r="H109" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J109" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>253</v>
       </c>
       <c r="B110" t="s">
         <v>254</v>
       </c>
-      <c r="G110" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I110" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C110" t="s">
+        <v>316</v>
+      </c>
+      <c r="H110" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J110" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>255</v>
       </c>
       <c r="B111" t="s">
         <v>256</v>
       </c>
-      <c r="G111" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I111" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>316</v>
+      </c>
+      <c r="H111" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J111" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>257</v>
       </c>
       <c r="B112" t="s">
         <v>258</v>
       </c>
-      <c r="G112" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I112" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C112" t="s">
+        <v>316</v>
+      </c>
+      <c r="H112" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J112" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>259</v>
       </c>
       <c r="B113" t="s">
         <v>260</v>
       </c>
-      <c r="G113" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I113" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C113" t="s">
+        <v>316</v>
+      </c>
+      <c r="H113" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J113" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>261</v>
       </c>
       <c r="B114" t="s">
         <v>262</v>
       </c>
-      <c r="G114" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I114" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C114" t="s">
+        <v>316</v>
+      </c>
+      <c r="H114" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J114" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>263</v>
       </c>
       <c r="B115" t="s">
         <v>264</v>
       </c>
-      <c r="G115" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I115" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C115" t="s">
+        <v>316</v>
+      </c>
+      <c r="H115" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J115" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>265</v>
       </c>
       <c r="B116" t="s">
         <v>266</v>
       </c>
-      <c r="G116" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I116" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C116" t="s">
+        <v>316</v>
+      </c>
+      <c r="H116" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J116" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>267</v>
       </c>
       <c r="B117" t="s">
         <v>268</v>
       </c>
-      <c r="G117" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I117" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>316</v>
+      </c>
+      <c r="H117" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J117" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>269</v>
       </c>
       <c r="B118" t="s">
         <v>270</v>
       </c>
-      <c r="G118" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I118" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>316</v>
+      </c>
+      <c r="H118" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J118" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>271</v>
       </c>
       <c r="B119" t="s">
         <v>272</v>
       </c>
-      <c r="G119" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I119" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>316</v>
+      </c>
+      <c r="H119" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J119" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>273</v>
       </c>
       <c r="B120" t="s">
         <v>274</v>
       </c>
-      <c r="G120" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I120" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>316</v>
+      </c>
+      <c r="H120" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J120" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>275</v>
       </c>
       <c r="B121" t="s">
         <v>276</v>
       </c>
-      <c r="G121" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I121" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>316</v>
+      </c>
+      <c r="H121" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J121" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>277</v>
       </c>
       <c r="B122" t="s">
         <v>278</v>
       </c>
-      <c r="G122" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I122" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C122" t="s">
+        <v>316</v>
+      </c>
+      <c r="H122" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J122" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>279</v>
       </c>
       <c r="B123" t="s">
         <v>280</v>
       </c>
-      <c r="G123" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I123" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C123" t="s">
+        <v>316</v>
+      </c>
+      <c r="H123" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J123" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>281</v>
       </c>
       <c r="B124" t="s">
         <v>282</v>
       </c>
-      <c r="G124" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I124" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C124" t="s">
+        <v>316</v>
+      </c>
+      <c r="H124" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J124" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>283</v>
       </c>
       <c r="B125" t="s">
         <v>284</v>
       </c>
-      <c r="G125" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I125" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
+        <v>316</v>
+      </c>
+      <c r="H125" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J125" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>285</v>
       </c>
       <c r="B126" t="s">
         <v>286</v>
       </c>
-      <c r="G126" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I126" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C126" t="s">
+        <v>316</v>
+      </c>
+      <c r="H126" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J126" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>287</v>
       </c>
       <c r="B127" t="s">
         <v>288</v>
       </c>
-      <c r="G127" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I127" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C127" t="s">
+        <v>316</v>
+      </c>
+      <c r="H127" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J127" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>289</v>
       </c>
       <c r="B128" t="s">
         <v>290</v>
       </c>
-      <c r="G128" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I128" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
+        <v>316</v>
+      </c>
+      <c r="H128" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J128" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>291</v>
       </c>
       <c r="B129" t="s">
         <v>292</v>
       </c>
-      <c r="G129" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I129" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
+        <v>316</v>
+      </c>
+      <c r="H129" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J129" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>293</v>
       </c>
       <c r="B130" t="s">
         <v>294</v>
       </c>
-      <c r="G130" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I130" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
+        <v>316</v>
+      </c>
+      <c r="H130" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J130" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>295</v>
       </c>
       <c r="B131" t="s">
         <v>296</v>
       </c>
-      <c r="G131" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I131" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C131" t="s">
+        <v>316</v>
+      </c>
+      <c r="H131" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J131" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>297</v>
       </c>
       <c r="B132" t="s">
         <v>298</v>
       </c>
-      <c r="G132" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I132" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>316</v>
+      </c>
+      <c r="H132" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J132" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>299</v>
       </c>
       <c r="B133" t="s">
         <v>300</v>
       </c>
-      <c r="G133" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I133" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C133" t="s">
+        <v>316</v>
+      </c>
+      <c r="H133" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J133" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>301</v>
       </c>
       <c r="B134" t="s">
         <v>302</v>
       </c>
-      <c r="G134" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I134" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>316</v>
+      </c>
+      <c r="H134" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J134" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>303</v>
       </c>
       <c r="B135" t="s">
         <v>304</v>
       </c>
-      <c r="G135" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I135" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C135" t="s">
+        <v>316</v>
+      </c>
+      <c r="H135" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J135" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>305</v>
       </c>
       <c r="B136" t="s">
         <v>306</v>
       </c>
-      <c r="G136" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I136" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C136" t="s">
+        <v>316</v>
+      </c>
+      <c r="H136" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J136" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>307</v>
       </c>
       <c r="B137" t="s">
         <v>308</v>
       </c>
-      <c r="G137" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I137" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>316</v>
+      </c>
+      <c r="H137" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J137" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>309</v>
       </c>
       <c r="B138" t="s">
         <v>310</v>
       </c>
-      <c r="G138" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I138" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>316</v>
+      </c>
+      <c r="H138" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J138" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>311</v>
       </c>
       <c r="B139" t="s">
         <v>312</v>
       </c>
-      <c r="G139" s="11">
-        <v>10123</v>
-      </c>
-      <c r="I139" t="s">
+      <c r="C139" t="s">
+        <v>316</v>
+      </c>
+      <c r="H139" s="11">
+        <v>10123</v>
+      </c>
+      <c r="J139" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3389,7 +3813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B137"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A115" workbookViewId="0">
       <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added a Function to List Buildings by Category.
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -70,9 +70,6 @@
     <t>Animal Shelter</t>
   </si>
   <si>
-    <t>site_ID</t>
-  </si>
-  <si>
     <t>site_name</t>
   </si>
   <si>
@@ -977,6 +974,9 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>site_id</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1408,7 @@
   <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>3</v>
@@ -1463,681 +1463,681 @@
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>314</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
       <c r="C5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H5" s="11">
         <v>10123</v>
       </c>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
       <c r="C6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H6" s="11">
         <v>10123</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
       <c r="C7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H7" s="11">
         <v>10123</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
         <v>50</v>
       </c>
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
       <c r="C8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H8" s="11">
         <v>10123</v>
       </c>
       <c r="J8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
       <c r="C9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H9" s="11">
         <v>10123</v>
       </c>
       <c r="J9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
       <c r="C10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H10" s="11">
         <v>10123</v>
       </c>
       <c r="J10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
       <c r="C11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H11" s="11">
         <v>10123</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
         <v>58</v>
       </c>
-      <c r="B12" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H12" s="11">
         <v>10123</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" t="s">
         <v>60</v>
       </c>
-      <c r="B13" t="s">
-        <v>61</v>
-      </c>
       <c r="C13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H13" s="11">
         <v>10123</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
       <c r="C14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H14" s="11">
         <v>10123</v>
       </c>
       <c r="J14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H15" s="11">
         <v>10123</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
         <v>66</v>
       </c>
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
       <c r="C16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H16" s="11">
         <v>10123</v>
       </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
       <c r="C17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H17" s="11">
         <v>10123</v>
       </c>
       <c r="J17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" t="s">
-        <v>71</v>
-      </c>
       <c r="C18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H18" s="11">
         <v>10123</v>
       </c>
       <c r="J18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
       <c r="C19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H19" s="11">
         <v>10123</v>
       </c>
       <c r="J19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
         <v>74</v>
       </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
       <c r="C20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H20" s="11">
         <v>10123</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
         <v>76</v>
       </c>
-      <c r="B21" t="s">
-        <v>77</v>
-      </c>
       <c r="C21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H21" s="11">
         <v>10123</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" t="s">
         <v>78</v>
       </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
       <c r="C22" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H22" s="11">
         <v>10123</v>
       </c>
       <c r="J22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
         <v>80</v>
       </c>
-      <c r="B23" t="s">
-        <v>81</v>
-      </c>
       <c r="C23" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H23" s="11">
         <v>10123</v>
       </c>
       <c r="J23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
       <c r="C24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H24" s="11">
         <v>10123</v>
       </c>
       <c r="J24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
         <v>84</v>
       </c>
-      <c r="B25" t="s">
-        <v>85</v>
-      </c>
       <c r="C25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H25" s="11">
         <v>10123</v>
       </c>
       <c r="J25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
         <v>86</v>
       </c>
-      <c r="B26" t="s">
-        <v>87</v>
-      </c>
       <c r="C26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H26" s="11">
         <v>10123</v>
       </c>
       <c r="J26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" t="s">
         <v>88</v>
       </c>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
       <c r="C27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H27" s="11">
         <v>10123</v>
       </c>
       <c r="J27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
         <v>90</v>
       </c>
-      <c r="B28" t="s">
-        <v>91</v>
-      </c>
       <c r="C28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H28" s="11">
         <v>10123</v>
       </c>
       <c r="J28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" t="s">
         <v>92</v>
       </c>
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
       <c r="C29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H29" s="11">
         <v>10123</v>
       </c>
       <c r="J29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" t="s">
         <v>94</v>
       </c>
-      <c r="B30" t="s">
-        <v>95</v>
-      </c>
       <c r="C30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H30" s="11">
         <v>10123</v>
       </c>
       <c r="J30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" t="s">
         <v>96</v>
       </c>
-      <c r="B31" t="s">
-        <v>97</v>
-      </c>
       <c r="C31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H31" s="11">
         <v>10123</v>
       </c>
       <c r="J31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" t="s">
         <v>98</v>
       </c>
-      <c r="B32" t="s">
-        <v>99</v>
-      </c>
       <c r="C32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H32" s="11">
         <v>10123</v>
       </c>
       <c r="J32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
         <v>100</v>
       </c>
-      <c r="B33" t="s">
-        <v>101</v>
-      </c>
       <c r="C33" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H33" s="11">
         <v>10123</v>
       </c>
       <c r="J33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
         <v>102</v>
       </c>
-      <c r="B34" t="s">
-        <v>103</v>
-      </c>
       <c r="C34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H34" s="11">
         <v>10123</v>
       </c>
       <c r="J34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
         <v>104</v>
       </c>
-      <c r="B35" t="s">
-        <v>105</v>
-      </c>
       <c r="C35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H35" s="11">
         <v>10123</v>
       </c>
       <c r="J35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
         <v>106</v>
       </c>
-      <c r="B36" t="s">
-        <v>107</v>
-      </c>
       <c r="C36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H36" s="11">
         <v>10123</v>
       </c>
       <c r="J36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
         <v>108</v>
       </c>
-      <c r="B37" t="s">
-        <v>109</v>
-      </c>
       <c r="C37" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H37" s="11">
         <v>10123</v>
       </c>
       <c r="J37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" t="s">
         <v>110</v>
       </c>
-      <c r="B38" t="s">
-        <v>111</v>
-      </c>
       <c r="C38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H38" s="11">
         <v>10123</v>
       </c>
       <c r="J38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s">
         <v>112</v>
       </c>
-      <c r="B39" t="s">
-        <v>113</v>
-      </c>
       <c r="C39" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H39" s="11">
         <v>10123</v>
       </c>
       <c r="J39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B40" t="s">
         <v>114</v>
       </c>
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
       <c r="C40" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H40" s="11">
         <v>10123</v>
       </c>
       <c r="J40" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" t="s">
         <v>116</v>
       </c>
-      <c r="B41" t="s">
-        <v>117</v>
-      </c>
       <c r="C41" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H41" s="11">
         <v>10123</v>
       </c>
       <c r="J41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" t="s">
         <v>118</v>
       </c>
-      <c r="B42" t="s">
-        <v>119</v>
-      </c>
       <c r="C42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H42" s="11">
         <v>10123</v>
       </c>
       <c r="J42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2145,10 +2145,10 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D43" t="s">
         <v>11</v>
@@ -2166,1639 +2166,1639 @@
         <v>10123</v>
       </c>
       <c r="J43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="B44" t="s">
-        <v>122</v>
-      </c>
       <c r="C44" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H44" s="11">
         <v>10123</v>
       </c>
       <c r="J44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" t="s">
         <v>123</v>
       </c>
-      <c r="B45" t="s">
-        <v>124</v>
-      </c>
       <c r="C45" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H45" s="11">
         <v>10123</v>
       </c>
       <c r="J45" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
         <v>125</v>
       </c>
-      <c r="B46" t="s">
-        <v>126</v>
-      </c>
       <c r="C46" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H46" s="11">
         <v>10123</v>
       </c>
       <c r="J46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" t="s">
         <v>127</v>
       </c>
-      <c r="B47" t="s">
-        <v>128</v>
-      </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H47" s="11">
         <v>10123</v>
       </c>
       <c r="J47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" t="s">
         <v>129</v>
       </c>
-      <c r="B48" t="s">
-        <v>130</v>
-      </c>
       <c r="C48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H48" s="11">
         <v>10123</v>
       </c>
       <c r="J48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>130</v>
+      </c>
+      <c r="B49" t="s">
         <v>131</v>
       </c>
-      <c r="B49" t="s">
-        <v>132</v>
-      </c>
       <c r="C49" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H49" s="11">
         <v>10123</v>
       </c>
       <c r="J49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>132</v>
+      </c>
+      <c r="B50" t="s">
         <v>133</v>
       </c>
-      <c r="B50" t="s">
-        <v>134</v>
-      </c>
       <c r="C50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H50" s="11">
         <v>10123</v>
       </c>
       <c r="J50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
         <v>135</v>
       </c>
-      <c r="B51" t="s">
-        <v>136</v>
-      </c>
       <c r="C51" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H51" s="11">
         <v>10123</v>
       </c>
       <c r="J51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" t="s">
         <v>137</v>
       </c>
-      <c r="B52" t="s">
-        <v>138</v>
-      </c>
       <c r="C52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H52" s="11">
         <v>10123</v>
       </c>
       <c r="J52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" t="s">
         <v>139</v>
       </c>
-      <c r="B53" t="s">
-        <v>140</v>
-      </c>
       <c r="C53" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H53" s="11">
         <v>10123</v>
       </c>
       <c r="J53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" t="s">
         <v>141</v>
       </c>
-      <c r="B54" t="s">
-        <v>142</v>
-      </c>
       <c r="C54" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H54" s="11">
         <v>10123</v>
       </c>
       <c r="J54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" t="s">
         <v>143</v>
       </c>
-      <c r="B55" t="s">
-        <v>144</v>
-      </c>
       <c r="C55" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H55" s="11">
         <v>10123</v>
       </c>
       <c r="J55" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" t="s">
         <v>145</v>
       </c>
-      <c r="B56" t="s">
-        <v>146</v>
-      </c>
       <c r="C56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H56" s="11">
         <v>10123</v>
       </c>
       <c r="J56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>146</v>
+      </c>
+      <c r="B57" t="s">
         <v>147</v>
       </c>
-      <c r="B57" t="s">
-        <v>148</v>
-      </c>
       <c r="C57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H57" s="11">
         <v>10123</v>
       </c>
       <c r="J57" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>148</v>
+      </c>
+      <c r="B58" t="s">
         <v>149</v>
       </c>
-      <c r="B58" t="s">
-        <v>150</v>
-      </c>
       <c r="C58" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H58" s="11">
         <v>10123</v>
       </c>
       <c r="J58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" t="s">
         <v>151</v>
       </c>
-      <c r="B59" t="s">
-        <v>152</v>
-      </c>
       <c r="C59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H59" s="11">
         <v>10123</v>
       </c>
       <c r="J59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" t="s">
         <v>153</v>
       </c>
-      <c r="B60" t="s">
-        <v>154</v>
-      </c>
       <c r="C60" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H60" s="11">
         <v>10123</v>
       </c>
       <c r="J60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" t="s">
         <v>155</v>
       </c>
-      <c r="B61" t="s">
-        <v>156</v>
-      </c>
       <c r="C61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H61" s="11">
         <v>10123</v>
       </c>
       <c r="J61" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" t="s">
         <v>157</v>
       </c>
-      <c r="B62" t="s">
-        <v>158</v>
-      </c>
       <c r="C62" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H62" s="11">
         <v>10123</v>
       </c>
       <c r="J62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" t="s">
         <v>159</v>
       </c>
-      <c r="B63" t="s">
-        <v>160</v>
-      </c>
       <c r="C63" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H63" s="11">
         <v>10123</v>
       </c>
       <c r="J63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>160</v>
+      </c>
+      <c r="B64" t="s">
         <v>161</v>
       </c>
-      <c r="B64" t="s">
-        <v>162</v>
-      </c>
       <c r="C64" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H64" s="11">
         <v>10123</v>
       </c>
       <c r="J64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>162</v>
+      </c>
+      <c r="B65" t="s">
         <v>163</v>
       </c>
-      <c r="B65" t="s">
-        <v>164</v>
-      </c>
       <c r="C65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H65" s="11">
         <v>10123</v>
       </c>
       <c r="J65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" t="s">
         <v>165</v>
       </c>
-      <c r="B66" t="s">
-        <v>166</v>
-      </c>
       <c r="C66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H66" s="11">
         <v>10123</v>
       </c>
       <c r="J66" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" t="s">
         <v>167</v>
       </c>
-      <c r="B67" t="s">
-        <v>168</v>
-      </c>
       <c r="C67" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H67" s="11">
         <v>10123</v>
       </c>
       <c r="J67" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" t="s">
         <v>169</v>
       </c>
-      <c r="B68" t="s">
-        <v>170</v>
-      </c>
       <c r="C68" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H68" s="11">
         <v>10123</v>
       </c>
       <c r="J68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>170</v>
+      </c>
+      <c r="B69" t="s">
         <v>171</v>
       </c>
-      <c r="B69" t="s">
-        <v>172</v>
-      </c>
       <c r="C69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H69" s="11">
         <v>10123</v>
       </c>
       <c r="J69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" t="s">
         <v>173</v>
       </c>
-      <c r="B70" t="s">
-        <v>174</v>
-      </c>
       <c r="C70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H70" s="11">
         <v>10123</v>
       </c>
       <c r="J70" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>174</v>
+      </c>
+      <c r="B71" t="s">
         <v>175</v>
       </c>
-      <c r="B71" t="s">
-        <v>176</v>
-      </c>
       <c r="C71" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H71" s="11">
         <v>10123</v>
       </c>
       <c r="J71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>176</v>
+      </c>
+      <c r="B72" t="s">
         <v>177</v>
       </c>
-      <c r="B72" t="s">
-        <v>178</v>
-      </c>
       <c r="C72" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H72" s="11">
         <v>10123</v>
       </c>
       <c r="J72" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>178</v>
+      </c>
+      <c r="B73" t="s">
         <v>179</v>
       </c>
-      <c r="B73" t="s">
-        <v>180</v>
-      </c>
       <c r="C73" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H73" s="11">
         <v>10123</v>
       </c>
       <c r="J73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>180</v>
+      </c>
+      <c r="B74" t="s">
         <v>181</v>
       </c>
-      <c r="B74" t="s">
-        <v>182</v>
-      </c>
       <c r="C74" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H74" s="11">
         <v>10123</v>
       </c>
       <c r="J74" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" t="s">
         <v>183</v>
       </c>
-      <c r="B75" t="s">
-        <v>184</v>
-      </c>
       <c r="C75" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H75" s="11">
         <v>10123</v>
       </c>
       <c r="J75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>184</v>
+      </c>
+      <c r="B76" t="s">
         <v>185</v>
       </c>
-      <c r="B76" t="s">
-        <v>186</v>
-      </c>
       <c r="C76" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H76" s="11">
         <v>10123</v>
       </c>
       <c r="J76" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>186</v>
+      </c>
+      <c r="B77" t="s">
         <v>187</v>
       </c>
-      <c r="B77" t="s">
-        <v>188</v>
-      </c>
       <c r="C77" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H77" s="11">
         <v>10123</v>
       </c>
       <c r="J77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>188</v>
+      </c>
+      <c r="B78" t="s">
         <v>189</v>
       </c>
-      <c r="B78" t="s">
-        <v>190</v>
-      </c>
       <c r="C78" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H78" s="11">
         <v>10123</v>
       </c>
       <c r="J78" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>190</v>
+      </c>
+      <c r="B79" t="s">
         <v>191</v>
       </c>
-      <c r="B79" t="s">
-        <v>192</v>
-      </c>
       <c r="C79" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H79" s="11">
         <v>10123</v>
       </c>
       <c r="J79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>192</v>
+      </c>
+      <c r="B80" t="s">
         <v>193</v>
       </c>
-      <c r="B80" t="s">
-        <v>194</v>
-      </c>
       <c r="C80" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H80" s="11">
         <v>10123</v>
       </c>
       <c r="J80" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>194</v>
+      </c>
+      <c r="B81" t="s">
         <v>195</v>
       </c>
-      <c r="B81" t="s">
-        <v>196</v>
-      </c>
       <c r="C81" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H81" s="11">
         <v>10123</v>
       </c>
       <c r="J81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>196</v>
+      </c>
+      <c r="B82" t="s">
         <v>197</v>
       </c>
-      <c r="B82" t="s">
-        <v>198</v>
-      </c>
       <c r="C82" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H82" s="11">
         <v>10123</v>
       </c>
       <c r="J82" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>198</v>
+      </c>
+      <c r="B83" t="s">
         <v>199</v>
       </c>
-      <c r="B83" t="s">
-        <v>200</v>
-      </c>
       <c r="C83" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H83" s="11">
         <v>10123</v>
       </c>
       <c r="J83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>200</v>
+      </c>
+      <c r="B84" t="s">
         <v>201</v>
       </c>
-      <c r="B84" t="s">
-        <v>202</v>
-      </c>
       <c r="C84" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H84" s="11">
         <v>10123</v>
       </c>
       <c r="J84" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>202</v>
+      </c>
+      <c r="B85" t="s">
         <v>203</v>
       </c>
-      <c r="B85" t="s">
-        <v>204</v>
-      </c>
       <c r="C85" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H85" s="11">
         <v>10123</v>
       </c>
       <c r="J85" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>204</v>
+      </c>
+      <c r="B86" t="s">
         <v>205</v>
       </c>
-      <c r="B86" t="s">
-        <v>206</v>
-      </c>
       <c r="C86" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H86" s="11">
         <v>10123</v>
       </c>
       <c r="J86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>206</v>
+      </c>
+      <c r="B87" t="s">
         <v>207</v>
       </c>
-      <c r="B87" t="s">
-        <v>208</v>
-      </c>
       <c r="C87" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H87" s="11">
         <v>10123</v>
       </c>
       <c r="J87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>208</v>
+      </c>
+      <c r="B88" t="s">
         <v>209</v>
       </c>
-      <c r="B88" t="s">
-        <v>210</v>
-      </c>
       <c r="C88" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H88" s="11">
         <v>10123</v>
       </c>
       <c r="J88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>210</v>
+      </c>
+      <c r="B89" t="s">
         <v>211</v>
       </c>
-      <c r="B89" t="s">
-        <v>212</v>
-      </c>
       <c r="C89" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H89" s="11">
         <v>10123</v>
       </c>
       <c r="J89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>212</v>
+      </c>
+      <c r="B90" t="s">
         <v>213</v>
       </c>
-      <c r="B90" t="s">
-        <v>214</v>
-      </c>
       <c r="C90" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H90" s="11">
         <v>10123</v>
       </c>
       <c r="J90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>214</v>
+      </c>
+      <c r="B91" t="s">
         <v>215</v>
       </c>
-      <c r="B91" t="s">
-        <v>216</v>
-      </c>
       <c r="C91" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H91" s="11">
         <v>10123</v>
       </c>
       <c r="J91" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>216</v>
+      </c>
+      <c r="B92" t="s">
         <v>217</v>
       </c>
-      <c r="B92" t="s">
-        <v>218</v>
-      </c>
       <c r="C92" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H92" s="11">
         <v>10123</v>
       </c>
       <c r="J92" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93" t="s">
         <v>219</v>
       </c>
-      <c r="B93" t="s">
-        <v>220</v>
-      </c>
       <c r="C93" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H93" s="11">
         <v>10123</v>
       </c>
       <c r="J93" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>220</v>
+      </c>
+      <c r="B94" t="s">
         <v>221</v>
       </c>
-      <c r="B94" t="s">
-        <v>222</v>
-      </c>
       <c r="C94" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H94" s="11">
         <v>10123</v>
       </c>
       <c r="J94" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>222</v>
+      </c>
+      <c r="B95" t="s">
         <v>223</v>
       </c>
-      <c r="B95" t="s">
-        <v>224</v>
-      </c>
       <c r="C95" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H95" s="11">
         <v>10123</v>
       </c>
       <c r="J95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>224</v>
+      </c>
+      <c r="B96" t="s">
         <v>225</v>
       </c>
-      <c r="B96" t="s">
-        <v>226</v>
-      </c>
       <c r="C96" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H96" s="11">
         <v>10123</v>
       </c>
       <c r="J96" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>226</v>
+      </c>
+      <c r="B97" t="s">
         <v>227</v>
       </c>
-      <c r="B97" t="s">
-        <v>228</v>
-      </c>
       <c r="C97" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H97" s="11">
         <v>10123</v>
       </c>
       <c r="J97" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>228</v>
+      </c>
+      <c r="B98" t="s">
         <v>229</v>
       </c>
-      <c r="B98" t="s">
-        <v>230</v>
-      </c>
       <c r="C98" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H98" s="11">
         <v>10123</v>
       </c>
       <c r="J98" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>230</v>
+      </c>
+      <c r="B99" t="s">
         <v>231</v>
       </c>
-      <c r="B99" t="s">
-        <v>232</v>
-      </c>
       <c r="C99" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H99" s="11">
         <v>10123</v>
       </c>
       <c r="J99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>232</v>
+      </c>
+      <c r="B100" t="s">
         <v>233</v>
       </c>
-      <c r="B100" t="s">
-        <v>234</v>
-      </c>
       <c r="C100" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H100" s="11">
         <v>10123</v>
       </c>
       <c r="J100" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>234</v>
+      </c>
+      <c r="B101" t="s">
         <v>235</v>
       </c>
-      <c r="B101" t="s">
-        <v>236</v>
-      </c>
       <c r="C101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H101" s="11">
         <v>10123</v>
       </c>
       <c r="J101" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>236</v>
+      </c>
+      <c r="B102" t="s">
         <v>237</v>
       </c>
-      <c r="B102" t="s">
-        <v>238</v>
-      </c>
       <c r="C102" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H102" s="11">
         <v>10123</v>
       </c>
       <c r="J102" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>238</v>
+      </c>
+      <c r="B103" t="s">
         <v>239</v>
       </c>
-      <c r="B103" t="s">
-        <v>240</v>
-      </c>
       <c r="C103" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H103" s="11">
         <v>10123</v>
       </c>
       <c r="J103" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
+        <v>240</v>
+      </c>
+      <c r="B104" t="s">
         <v>241</v>
       </c>
-      <c r="B104" t="s">
-        <v>242</v>
-      </c>
       <c r="C104" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H104" s="11">
         <v>10123</v>
       </c>
       <c r="J104" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>242</v>
+      </c>
+      <c r="B105" t="s">
         <v>243</v>
       </c>
-      <c r="B105" t="s">
-        <v>244</v>
-      </c>
       <c r="C105" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H105" s="11">
         <v>10123</v>
       </c>
       <c r="J105" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>244</v>
+      </c>
+      <c r="B106" t="s">
         <v>245</v>
       </c>
-      <c r="B106" t="s">
-        <v>246</v>
-      </c>
       <c r="C106" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H106" s="11">
         <v>10123</v>
       </c>
       <c r="J106" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>246</v>
+      </c>
+      <c r="B107" t="s">
         <v>247</v>
       </c>
-      <c r="B107" t="s">
-        <v>248</v>
-      </c>
       <c r="C107" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H107" s="11">
         <v>10123</v>
       </c>
       <c r="J107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>248</v>
+      </c>
+      <c r="B108" t="s">
         <v>249</v>
       </c>
-      <c r="B108" t="s">
-        <v>250</v>
-      </c>
       <c r="C108" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H108" s="11">
         <v>10123</v>
       </c>
       <c r="J108" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>250</v>
+      </c>
+      <c r="B109" t="s">
         <v>251</v>
       </c>
-      <c r="B109" t="s">
-        <v>252</v>
-      </c>
       <c r="C109" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H109" s="11">
         <v>10123</v>
       </c>
       <c r="J109" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>252</v>
+      </c>
+      <c r="B110" t="s">
         <v>253</v>
       </c>
-      <c r="B110" t="s">
-        <v>254</v>
-      </c>
       <c r="C110" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H110" s="11">
         <v>10123</v>
       </c>
       <c r="J110" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>254</v>
+      </c>
+      <c r="B111" t="s">
         <v>255</v>
       </c>
-      <c r="B111" t="s">
-        <v>256</v>
-      </c>
       <c r="C111" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H111" s="11">
         <v>10123</v>
       </c>
       <c r="J111" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>256</v>
+      </c>
+      <c r="B112" t="s">
         <v>257</v>
       </c>
-      <c r="B112" t="s">
-        <v>258</v>
-      </c>
       <c r="C112" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H112" s="11">
         <v>10123</v>
       </c>
       <c r="J112" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>258</v>
+      </c>
+      <c r="B113" t="s">
         <v>259</v>
       </c>
-      <c r="B113" t="s">
-        <v>260</v>
-      </c>
       <c r="C113" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H113" s="11">
         <v>10123</v>
       </c>
       <c r="J113" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>260</v>
+      </c>
+      <c r="B114" t="s">
         <v>261</v>
       </c>
-      <c r="B114" t="s">
-        <v>262</v>
-      </c>
       <c r="C114" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H114" s="11">
         <v>10123</v>
       </c>
       <c r="J114" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>262</v>
+      </c>
+      <c r="B115" t="s">
         <v>263</v>
       </c>
-      <c r="B115" t="s">
-        <v>264</v>
-      </c>
       <c r="C115" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H115" s="11">
         <v>10123</v>
       </c>
       <c r="J115" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>264</v>
+      </c>
+      <c r="B116" t="s">
         <v>265</v>
       </c>
-      <c r="B116" t="s">
-        <v>266</v>
-      </c>
       <c r="C116" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H116" s="11">
         <v>10123</v>
       </c>
       <c r="J116" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>266</v>
+      </c>
+      <c r="B117" t="s">
         <v>267</v>
       </c>
-      <c r="B117" t="s">
-        <v>268</v>
-      </c>
       <c r="C117" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H117" s="11">
         <v>10123</v>
       </c>
       <c r="J117" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>268</v>
+      </c>
+      <c r="B118" t="s">
         <v>269</v>
       </c>
-      <c r="B118" t="s">
-        <v>270</v>
-      </c>
       <c r="C118" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H118" s="11">
         <v>10123</v>
       </c>
       <c r="J118" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>270</v>
+      </c>
+      <c r="B119" t="s">
         <v>271</v>
       </c>
-      <c r="B119" t="s">
-        <v>272</v>
-      </c>
       <c r="C119" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H119" s="11">
         <v>10123</v>
       </c>
       <c r="J119" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>272</v>
+      </c>
+      <c r="B120" t="s">
         <v>273</v>
       </c>
-      <c r="B120" t="s">
-        <v>274</v>
-      </c>
       <c r="C120" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H120" s="11">
         <v>10123</v>
       </c>
       <c r="J120" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>274</v>
+      </c>
+      <c r="B121" t="s">
         <v>275</v>
       </c>
-      <c r="B121" t="s">
-        <v>276</v>
-      </c>
       <c r="C121" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H121" s="11">
         <v>10123</v>
       </c>
       <c r="J121" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>276</v>
+      </c>
+      <c r="B122" t="s">
         <v>277</v>
       </c>
-      <c r="B122" t="s">
-        <v>278</v>
-      </c>
       <c r="C122" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H122" s="11">
         <v>10123</v>
       </c>
       <c r="J122" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>278</v>
+      </c>
+      <c r="B123" t="s">
         <v>279</v>
       </c>
-      <c r="B123" t="s">
-        <v>280</v>
-      </c>
       <c r="C123" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H123" s="11">
         <v>10123</v>
       </c>
       <c r="J123" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>280</v>
+      </c>
+      <c r="B124" t="s">
         <v>281</v>
       </c>
-      <c r="B124" t="s">
-        <v>282</v>
-      </c>
       <c r="C124" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H124" s="11">
         <v>10123</v>
       </c>
       <c r="J124" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>282</v>
+      </c>
+      <c r="B125" t="s">
         <v>283</v>
       </c>
-      <c r="B125" t="s">
-        <v>284</v>
-      </c>
       <c r="C125" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H125" s="11">
         <v>10123</v>
       </c>
       <c r="J125" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>284</v>
+      </c>
+      <c r="B126" t="s">
         <v>285</v>
       </c>
-      <c r="B126" t="s">
-        <v>286</v>
-      </c>
       <c r="C126" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H126" s="11">
         <v>10123</v>
       </c>
       <c r="J126" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>286</v>
+      </c>
+      <c r="B127" t="s">
         <v>287</v>
       </c>
-      <c r="B127" t="s">
-        <v>288</v>
-      </c>
       <c r="C127" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H127" s="11">
         <v>10123</v>
       </c>
       <c r="J127" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>288</v>
+      </c>
+      <c r="B128" t="s">
         <v>289</v>
       </c>
-      <c r="B128" t="s">
-        <v>290</v>
-      </c>
       <c r="C128" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H128" s="11">
         <v>10123</v>
       </c>
       <c r="J128" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>290</v>
+      </c>
+      <c r="B129" t="s">
         <v>291</v>
       </c>
-      <c r="B129" t="s">
-        <v>292</v>
-      </c>
       <c r="C129" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H129" s="11">
         <v>10123</v>
       </c>
       <c r="J129" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>292</v>
+      </c>
+      <c r="B130" t="s">
         <v>293</v>
       </c>
-      <c r="B130" t="s">
-        <v>294</v>
-      </c>
       <c r="C130" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H130" s="11">
         <v>10123</v>
       </c>
       <c r="J130" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>294</v>
+      </c>
+      <c r="B131" t="s">
         <v>295</v>
       </c>
-      <c r="B131" t="s">
-        <v>296</v>
-      </c>
       <c r="C131" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H131" s="11">
         <v>10123</v>
       </c>
       <c r="J131" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>296</v>
+      </c>
+      <c r="B132" t="s">
         <v>297</v>
       </c>
-      <c r="B132" t="s">
-        <v>298</v>
-      </c>
       <c r="C132" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H132" s="11">
         <v>10123</v>
       </c>
       <c r="J132" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>298</v>
+      </c>
+      <c r="B133" t="s">
         <v>299</v>
       </c>
-      <c r="B133" t="s">
-        <v>300</v>
-      </c>
       <c r="C133" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H133" s="11">
         <v>10123</v>
       </c>
       <c r="J133" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>300</v>
+      </c>
+      <c r="B134" t="s">
         <v>301</v>
       </c>
-      <c r="B134" t="s">
-        <v>302</v>
-      </c>
       <c r="C134" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H134" s="11">
         <v>10123</v>
       </c>
       <c r="J134" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
+        <v>302</v>
+      </c>
+      <c r="B135" t="s">
         <v>303</v>
       </c>
-      <c r="B135" t="s">
-        <v>304</v>
-      </c>
       <c r="C135" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H135" s="11">
         <v>10123</v>
       </c>
       <c r="J135" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
+        <v>304</v>
+      </c>
+      <c r="B136" t="s">
         <v>305</v>
       </c>
-      <c r="B136" t="s">
-        <v>306</v>
-      </c>
       <c r="C136" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H136" s="11">
         <v>10123</v>
       </c>
       <c r="J136" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>306</v>
+      </c>
+      <c r="B137" t="s">
         <v>307</v>
       </c>
-      <c r="B137" t="s">
-        <v>308</v>
-      </c>
       <c r="C137" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H137" s="11">
         <v>10123</v>
       </c>
       <c r="J137" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
+        <v>308</v>
+      </c>
+      <c r="B138" t="s">
         <v>309</v>
       </c>
-      <c r="B138" t="s">
-        <v>310</v>
-      </c>
       <c r="C138" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H138" s="11">
         <v>10123</v>
       </c>
       <c r="J138" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>310</v>
+      </c>
+      <c r="B139" t="s">
         <v>311</v>
       </c>
-      <c r="B139" t="s">
-        <v>312</v>
-      </c>
       <c r="C139" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H139" s="11">
         <v>10123</v>
       </c>
       <c r="J139" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3821,20 +3821,20 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4898,38 +4898,38 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
       </c>
       <c r="C5" s="2">
         <v>102000</v>
@@ -4937,10 +4937,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
       </c>
       <c r="C6" s="2">
         <v>3412</v>
@@ -4948,10 +4948,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2">
         <v>135000</v>
@@ -4959,10 +4959,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
       </c>
       <c r="C8" s="2">
         <v>1000000</v>
@@ -4970,10 +4970,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2">
         <v>1194000</v>
@@ -4981,10 +4981,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2">
         <v>1194</v>

</xml_diff>

<commit_message>
Other Data with Real Square Feet Values
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26760" windowHeight="11070"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Building" sheetId="1" r:id="rId1"/>
@@ -985,7 +985,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1067,10 +1067,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1090,6 +1090,7 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1408,7 +1409,7 @@
   <dimension ref="A1:L139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1419,7 @@
     <col min="4" max="4" width="33.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" customWidth="1"/>
     <col min="9" max="9" width="29.5703125" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
@@ -1504,8 +1505,9 @@
       <c r="C5" t="s">
         <v>314</v>
       </c>
+      <c r="G5" s="12"/>
       <c r="H5" s="11">
-        <v>10123</v>
+        <v>49210</v>
       </c>
       <c r="J5" t="s">
         <v>34</v>
@@ -1521,8 +1523,9 @@
       <c r="C6" t="s">
         <v>314</v>
       </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="11">
-        <v>10123</v>
+        <v>49210</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
@@ -1538,8 +1541,9 @@
       <c r="C7" t="s">
         <v>314</v>
       </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="11">
-        <v>10123</v>
+        <v>234412</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
@@ -1555,8 +1559,9 @@
       <c r="C8" t="s">
         <v>314</v>
       </c>
+      <c r="G8" s="12"/>
       <c r="H8" s="11">
-        <v>10123</v>
+        <v>57047</v>
       </c>
       <c r="J8" t="s">
         <v>34</v>
@@ -1572,8 +1577,9 @@
       <c r="C9" t="s">
         <v>314</v>
       </c>
+      <c r="G9" s="12"/>
       <c r="H9" s="11">
-        <v>10123</v>
+        <v>64699</v>
       </c>
       <c r="J9" t="s">
         <v>34</v>
@@ -1589,8 +1595,9 @@
       <c r="C10" t="s">
         <v>314</v>
       </c>
+      <c r="G10" s="12"/>
       <c r="H10" s="11">
-        <v>10123</v>
+        <v>74654</v>
       </c>
       <c r="J10" t="s">
         <v>34</v>
@@ -1606,8 +1613,9 @@
       <c r="C11" t="s">
         <v>314</v>
       </c>
+      <c r="G11" s="12"/>
       <c r="H11" s="11">
-        <v>10123</v>
+        <v>60642</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
@@ -1623,8 +1631,9 @@
       <c r="C12" t="s">
         <v>314</v>
       </c>
+      <c r="G12" s="12"/>
       <c r="H12" s="11">
-        <v>10123</v>
+        <v>13608</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
@@ -1640,8 +1649,9 @@
       <c r="C13" t="s">
         <v>314</v>
       </c>
+      <c r="G13" s="12"/>
       <c r="H13" s="11">
-        <v>10123</v>
+        <v>24496</v>
       </c>
       <c r="J13" t="s">
         <v>34</v>
@@ -1657,8 +1667,9 @@
       <c r="C14" t="s">
         <v>314</v>
       </c>
+      <c r="G14" s="12"/>
       <c r="H14" s="11">
-        <v>10123</v>
+        <v>81654</v>
       </c>
       <c r="J14" t="s">
         <v>34</v>
@@ -1674,8 +1685,9 @@
       <c r="C15" t="s">
         <v>314</v>
       </c>
+      <c r="G15" s="12"/>
       <c r="H15" s="11">
-        <v>10123</v>
+        <v>57154</v>
       </c>
       <c r="J15" t="s">
         <v>34</v>
@@ -1691,8 +1703,9 @@
       <c r="C16" t="s">
         <v>314</v>
       </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="11">
-        <v>10123</v>
+        <v>99880</v>
       </c>
       <c r="J16" t="s">
         <v>34</v>
@@ -1708,8 +1721,9 @@
       <c r="C17" t="s">
         <v>314</v>
       </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="11">
-        <v>10123</v>
+        <v>137524</v>
       </c>
       <c r="J17" t="s">
         <v>34</v>
@@ -1725,8 +1739,9 @@
       <c r="C18" t="s">
         <v>314</v>
       </c>
+      <c r="G18" s="12"/>
       <c r="H18" s="11">
-        <v>10123</v>
+        <v>32832</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
@@ -1742,8 +1757,9 @@
       <c r="C19" t="s">
         <v>314</v>
       </c>
-      <c r="H19" s="11">
-        <v>10123</v>
+      <c r="G19" s="12"/>
+      <c r="H19">
+        <v>0</v>
       </c>
       <c r="J19" t="s">
         <v>34</v>
@@ -1759,8 +1775,9 @@
       <c r="C20" t="s">
         <v>314</v>
       </c>
-      <c r="H20" s="11">
-        <v>10123</v>
+      <c r="G20" s="12"/>
+      <c r="H20">
+        <v>0</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
@@ -1776,8 +1793,9 @@
       <c r="C21" t="s">
         <v>314</v>
       </c>
+      <c r="G21" s="12"/>
       <c r="H21" s="11">
-        <v>10123</v>
+        <v>43996</v>
       </c>
       <c r="J21" t="s">
         <v>34</v>
@@ -1793,8 +1811,9 @@
       <c r="C22" t="s">
         <v>314</v>
       </c>
+      <c r="G22" s="12"/>
       <c r="H22" s="11">
-        <v>10123</v>
+        <v>103200</v>
       </c>
       <c r="J22" t="s">
         <v>34</v>
@@ -1810,8 +1829,9 @@
       <c r="C23" t="s">
         <v>314</v>
       </c>
+      <c r="G23" s="12"/>
       <c r="H23" s="11">
-        <v>10123</v>
+        <v>113306</v>
       </c>
       <c r="J23" t="s">
         <v>34</v>
@@ -1827,8 +1847,9 @@
       <c r="C24" t="s">
         <v>314</v>
       </c>
+      <c r="G24" s="12"/>
       <c r="H24" s="11">
-        <v>10123</v>
+        <v>156362</v>
       </c>
       <c r="J24" t="s">
         <v>34</v>
@@ -1844,8 +1865,9 @@
       <c r="C25" t="s">
         <v>314</v>
       </c>
+      <c r="G25" s="12"/>
       <c r="H25" s="11">
-        <v>10123</v>
+        <v>101069</v>
       </c>
       <c r="J25" t="s">
         <v>34</v>
@@ -1861,8 +1883,9 @@
       <c r="C26" t="s">
         <v>314</v>
       </c>
+      <c r="G26" s="12"/>
       <c r="H26" s="11">
-        <v>10123</v>
+        <v>216884</v>
       </c>
       <c r="J26" t="s">
         <v>34</v>
@@ -1878,8 +1901,9 @@
       <c r="C27" t="s">
         <v>314</v>
       </c>
+      <c r="G27" s="12"/>
       <c r="H27" s="11">
-        <v>10123</v>
+        <v>64408</v>
       </c>
       <c r="J27" t="s">
         <v>34</v>
@@ -1895,8 +1919,9 @@
       <c r="C28" t="s">
         <v>314</v>
       </c>
+      <c r="G28" s="12"/>
       <c r="H28" s="11">
-        <v>10123</v>
+        <v>64458</v>
       </c>
       <c r="J28" t="s">
         <v>34</v>
@@ -1912,8 +1937,9 @@
       <c r="C29" t="s">
         <v>314</v>
       </c>
+      <c r="G29" s="12"/>
       <c r="H29" s="11">
-        <v>10123</v>
+        <v>62982</v>
       </c>
       <c r="J29" t="s">
         <v>34</v>
@@ -1929,8 +1955,9 @@
       <c r="C30" t="s">
         <v>314</v>
       </c>
+      <c r="G30" s="12"/>
       <c r="H30" s="11">
-        <v>10123</v>
+        <v>22200</v>
       </c>
       <c r="J30" t="s">
         <v>34</v>
@@ -1946,8 +1973,9 @@
       <c r="C31" t="s">
         <v>314</v>
       </c>
+      <c r="G31" s="12"/>
       <c r="H31" s="11">
-        <v>10123</v>
+        <v>65259</v>
       </c>
       <c r="J31" t="s">
         <v>34</v>
@@ -1963,8 +1991,9 @@
       <c r="C32" t="s">
         <v>314</v>
       </c>
+      <c r="G32" s="12"/>
       <c r="H32" s="11">
-        <v>10123</v>
+        <v>63761</v>
       </c>
       <c r="J32" t="s">
         <v>34</v>
@@ -1980,8 +2009,9 @@
       <c r="C33" t="s">
         <v>314</v>
       </c>
+      <c r="G33" s="12"/>
       <c r="H33" s="11">
-        <v>10123</v>
+        <v>30856</v>
       </c>
       <c r="J33" t="s">
         <v>34</v>
@@ -1997,8 +2027,9 @@
       <c r="C34" t="s">
         <v>314</v>
       </c>
+      <c r="G34" s="12"/>
       <c r="H34" s="11">
-        <v>10123</v>
+        <v>63455</v>
       </c>
       <c r="J34" t="s">
         <v>34</v>
@@ -2014,8 +2045,9 @@
       <c r="C35" t="s">
         <v>314</v>
       </c>
+      <c r="G35" s="12"/>
       <c r="H35" s="11">
-        <v>10123</v>
+        <v>68272</v>
       </c>
       <c r="J35" t="s">
         <v>34</v>
@@ -2031,8 +2063,9 @@
       <c r="C36" t="s">
         <v>314</v>
       </c>
+      <c r="G36" s="12"/>
       <c r="H36" s="11">
-        <v>10123</v>
+        <v>63532</v>
       </c>
       <c r="J36" t="s">
         <v>34</v>
@@ -2048,9 +2081,7 @@
       <c r="C37" t="s">
         <v>314</v>
       </c>
-      <c r="H37" s="11">
-        <v>10123</v>
-      </c>
+      <c r="G37" s="12"/>
       <c r="J37" t="s">
         <v>34</v>
       </c>
@@ -2065,8 +2096,9 @@
       <c r="C38" t="s">
         <v>314</v>
       </c>
+      <c r="G38" s="12"/>
       <c r="H38" s="11">
-        <v>10123</v>
+        <v>63532</v>
       </c>
       <c r="J38" t="s">
         <v>34</v>
@@ -2082,8 +2114,9 @@
       <c r="C39" t="s">
         <v>314</v>
       </c>
+      <c r="G39" s="12"/>
       <c r="H39" s="11">
-        <v>10123</v>
+        <v>74589</v>
       </c>
       <c r="J39" t="s">
         <v>34</v>
@@ -2099,9 +2132,7 @@
       <c r="C40" t="s">
         <v>314</v>
       </c>
-      <c r="H40" s="11">
-        <v>10123</v>
-      </c>
+      <c r="G40" s="12"/>
       <c r="J40" t="s">
         <v>34</v>
       </c>
@@ -2116,8 +2147,9 @@
       <c r="C41" t="s">
         <v>314</v>
       </c>
-      <c r="H41" s="11">
-        <v>10123</v>
+      <c r="G41" s="12"/>
+      <c r="H41">
+        <v>0</v>
       </c>
       <c r="J41" t="s">
         <v>34</v>
@@ -2133,8 +2165,9 @@
       <c r="C42" t="s">
         <v>315</v>
       </c>
-      <c r="H42" s="11">
-        <v>10123</v>
+      <c r="G42" s="12"/>
+      <c r="H42">
+        <v>0</v>
       </c>
       <c r="J42" t="s">
         <v>34</v>
@@ -2159,11 +2192,9 @@
       <c r="F43" t="s">
         <v>13</v>
       </c>
-      <c r="G43">
-        <v>1993</v>
-      </c>
+      <c r="G43" s="12"/>
       <c r="H43" s="11">
-        <v>10123</v>
+        <v>6718</v>
       </c>
       <c r="J43" t="s">
         <v>34</v>
@@ -2179,8 +2210,9 @@
       <c r="C44" t="s">
         <v>315</v>
       </c>
+      <c r="G44" s="12"/>
       <c r="H44" s="11">
-        <v>10123</v>
+        <v>2350</v>
       </c>
       <c r="J44" t="s">
         <v>34</v>
@@ -2196,8 +2228,9 @@
       <c r="C45" t="s">
         <v>315</v>
       </c>
-      <c r="H45" s="11">
-        <v>10123</v>
+      <c r="G45" s="12"/>
+      <c r="H45">
+        <v>0</v>
       </c>
       <c r="J45" t="s">
         <v>34</v>
@@ -2213,8 +2246,9 @@
       <c r="C46" t="s">
         <v>315</v>
       </c>
+      <c r="G46" s="12"/>
       <c r="H46" s="11">
-        <v>10123</v>
+        <v>1800</v>
       </c>
       <c r="J46" t="s">
         <v>34</v>
@@ -2230,8 +2264,9 @@
       <c r="C47" t="s">
         <v>315</v>
       </c>
-      <c r="H47" s="11">
-        <v>10123</v>
+      <c r="G47" s="12"/>
+      <c r="H47">
+        <v>242</v>
       </c>
       <c r="J47" t="s">
         <v>34</v>
@@ -2247,8 +2282,9 @@
       <c r="C48" t="s">
         <v>315</v>
       </c>
+      <c r="G48" s="12"/>
       <c r="H48" s="11">
-        <v>10123</v>
+        <v>2268</v>
       </c>
       <c r="J48" t="s">
         <v>34</v>
@@ -2264,8 +2300,9 @@
       <c r="C49" t="s">
         <v>315</v>
       </c>
+      <c r="G49" s="12"/>
       <c r="H49" s="11">
-        <v>10123</v>
+        <v>35500</v>
       </c>
       <c r="J49" t="s">
         <v>34</v>
@@ -2281,8 +2318,9 @@
       <c r="C50" t="s">
         <v>315</v>
       </c>
-      <c r="H50" s="11">
-        <v>10123</v>
+      <c r="G50" s="12"/>
+      <c r="H50">
+        <v>0</v>
       </c>
       <c r="J50" t="s">
         <v>34</v>
@@ -2298,8 +2336,9 @@
       <c r="C51" t="s">
         <v>315</v>
       </c>
-      <c r="H51" s="11">
-        <v>10123</v>
+      <c r="G51" s="12"/>
+      <c r="H51">
+        <v>0</v>
       </c>
       <c r="J51" t="s">
         <v>34</v>
@@ -2315,8 +2354,9 @@
       <c r="C52" t="s">
         <v>315</v>
       </c>
+      <c r="G52" s="12"/>
       <c r="H52" s="11">
-        <v>10123</v>
+        <v>13500</v>
       </c>
       <c r="J52" t="s">
         <v>34</v>
@@ -2332,8 +2372,9 @@
       <c r="C53" t="s">
         <v>315</v>
       </c>
-      <c r="H53" s="11">
-        <v>10123</v>
+      <c r="G53" s="12"/>
+      <c r="H53">
+        <v>0</v>
       </c>
       <c r="J53" t="s">
         <v>34</v>
@@ -2349,8 +2390,9 @@
       <c r="C54" t="s">
         <v>315</v>
       </c>
+      <c r="G54" s="12"/>
       <c r="H54" s="11">
-        <v>10123</v>
+        <v>2350</v>
       </c>
       <c r="J54" t="s">
         <v>34</v>
@@ -2366,8 +2408,9 @@
       <c r="C55" t="s">
         <v>315</v>
       </c>
+      <c r="G55" s="12"/>
       <c r="H55" s="11">
-        <v>10123</v>
+        <v>11188</v>
       </c>
       <c r="J55" t="s">
         <v>34</v>
@@ -2383,8 +2426,9 @@
       <c r="C56" t="s">
         <v>315</v>
       </c>
-      <c r="H56" s="11">
-        <v>10123</v>
+      <c r="G56" s="12"/>
+      <c r="H56">
+        <v>0</v>
       </c>
       <c r="J56" t="s">
         <v>34</v>
@@ -2400,8 +2444,9 @@
       <c r="C57" t="s">
         <v>315</v>
       </c>
-      <c r="H57" s="11">
-        <v>10123</v>
+      <c r="G57" s="12"/>
+      <c r="H57">
+        <v>0</v>
       </c>
       <c r="J57" t="s">
         <v>34</v>
@@ -2417,8 +2462,9 @@
       <c r="C58" t="s">
         <v>315</v>
       </c>
+      <c r="G58" s="12"/>
       <c r="H58" s="11">
-        <v>10123</v>
+        <v>5600</v>
       </c>
       <c r="J58" t="s">
         <v>34</v>
@@ -2434,8 +2480,9 @@
       <c r="C59" t="s">
         <v>315</v>
       </c>
+      <c r="G59" s="12"/>
       <c r="H59" s="11">
-        <v>10123</v>
+        <v>3742</v>
       </c>
       <c r="J59" t="s">
         <v>34</v>
@@ -2451,8 +2498,9 @@
       <c r="C60" t="s">
         <v>315</v>
       </c>
+      <c r="G60" s="12"/>
       <c r="H60" s="11">
-        <v>10123</v>
+        <v>34500</v>
       </c>
       <c r="J60" t="s">
         <v>34</v>
@@ -2468,8 +2516,9 @@
       <c r="C61" t="s">
         <v>315</v>
       </c>
+      <c r="G61" s="12"/>
       <c r="H61" s="11">
-        <v>10123</v>
+        <v>44892</v>
       </c>
       <c r="J61" t="s">
         <v>34</v>
@@ -2485,8 +2534,9 @@
       <c r="C62" t="s">
         <v>315</v>
       </c>
-      <c r="H62" s="11">
-        <v>10123</v>
+      <c r="G62" s="12"/>
+      <c r="H62">
+        <v>0</v>
       </c>
       <c r="J62" t="s">
         <v>34</v>
@@ -2502,8 +2552,9 @@
       <c r="C63" t="s">
         <v>315</v>
       </c>
-      <c r="H63" s="11">
-        <v>10123</v>
+      <c r="G63" s="12"/>
+      <c r="H63">
+        <v>440</v>
       </c>
       <c r="J63" t="s">
         <v>34</v>
@@ -2519,8 +2570,9 @@
       <c r="C64" t="s">
         <v>315</v>
       </c>
+      <c r="G64" s="12"/>
       <c r="H64" s="11">
-        <v>10123</v>
+        <v>1392</v>
       </c>
       <c r="J64" t="s">
         <v>34</v>
@@ -2536,8 +2588,9 @@
       <c r="C65" t="s">
         <v>315</v>
       </c>
+      <c r="G65" s="12"/>
       <c r="H65" s="11">
-        <v>10123</v>
+        <v>2620</v>
       </c>
       <c r="J65" t="s">
         <v>34</v>
@@ -2553,8 +2606,9 @@
       <c r="C66" t="s">
         <v>315</v>
       </c>
+      <c r="G66" s="12"/>
       <c r="H66" s="11">
-        <v>10123</v>
+        <v>1180</v>
       </c>
       <c r="J66" t="s">
         <v>34</v>
@@ -2570,8 +2624,9 @@
       <c r="C67" t="s">
         <v>315</v>
       </c>
+      <c r="G67" s="12"/>
       <c r="H67" s="11">
-        <v>10123</v>
+        <v>11175</v>
       </c>
       <c r="J67" t="s">
         <v>34</v>
@@ -2587,8 +2642,9 @@
       <c r="C68" t="s">
         <v>315</v>
       </c>
-      <c r="H68" s="11">
-        <v>10123</v>
+      <c r="G68" s="12"/>
+      <c r="H68">
+        <v>0</v>
       </c>
       <c r="J68" t="s">
         <v>34</v>
@@ -2604,8 +2660,9 @@
       <c r="C69" t="s">
         <v>315</v>
       </c>
-      <c r="H69" s="11">
-        <v>10123</v>
+      <c r="G69" s="12"/>
+      <c r="H69">
+        <v>0</v>
       </c>
       <c r="J69" t="s">
         <v>34</v>
@@ -2621,8 +2678,9 @@
       <c r="C70" t="s">
         <v>315</v>
       </c>
-      <c r="H70" s="11">
-        <v>10123</v>
+      <c r="G70" s="12"/>
+      <c r="H70">
+        <v>0</v>
       </c>
       <c r="J70" t="s">
         <v>34</v>
@@ -2638,8 +2696,9 @@
       <c r="C71" t="s">
         <v>315</v>
       </c>
-      <c r="H71" s="11">
-        <v>10123</v>
+      <c r="G71" s="12"/>
+      <c r="H71">
+        <v>0</v>
       </c>
       <c r="J71" t="s">
         <v>34</v>
@@ -2655,8 +2714,9 @@
       <c r="C72" t="s">
         <v>315</v>
       </c>
+      <c r="G72" s="12"/>
       <c r="H72" s="11">
-        <v>10123</v>
+        <v>118800</v>
       </c>
       <c r="J72" t="s">
         <v>34</v>
@@ -2672,8 +2732,9 @@
       <c r="C73" t="s">
         <v>315</v>
       </c>
-      <c r="H73" s="11">
-        <v>10123</v>
+      <c r="G73" s="12"/>
+      <c r="H73">
+        <v>0</v>
       </c>
       <c r="J73" t="s">
         <v>34</v>
@@ -2689,9 +2750,7 @@
       <c r="C74" t="s">
         <v>315</v>
       </c>
-      <c r="H74" s="11">
-        <v>10123</v>
-      </c>
+      <c r="G74" s="12"/>
       <c r="J74" t="s">
         <v>34</v>
       </c>
@@ -2706,8 +2765,9 @@
       <c r="C75" t="s">
         <v>315</v>
       </c>
-      <c r="H75" s="11">
-        <v>10123</v>
+      <c r="G75" s="12"/>
+      <c r="H75">
+        <v>0</v>
       </c>
       <c r="J75" t="s">
         <v>34</v>
@@ -2723,8 +2783,9 @@
       <c r="C76" t="s">
         <v>315</v>
       </c>
-      <c r="H76" s="11">
-        <v>10123</v>
+      <c r="G76" s="12"/>
+      <c r="H76">
+        <v>0</v>
       </c>
       <c r="J76" t="s">
         <v>34</v>
@@ -2740,8 +2801,9 @@
       <c r="C77" t="s">
         <v>315</v>
       </c>
-      <c r="H77" s="11">
-        <v>10123</v>
+      <c r="G77" s="12"/>
+      <c r="H77">
+        <v>0</v>
       </c>
       <c r="J77" t="s">
         <v>34</v>
@@ -2757,8 +2819,9 @@
       <c r="C78" t="s">
         <v>315</v>
       </c>
-      <c r="H78" s="11">
-        <v>10123</v>
+      <c r="G78" s="12"/>
+      <c r="H78">
+        <v>0</v>
       </c>
       <c r="J78" t="s">
         <v>34</v>
@@ -2774,8 +2837,9 @@
       <c r="C79" t="s">
         <v>315</v>
       </c>
-      <c r="H79" s="11">
-        <v>10123</v>
+      <c r="G79" s="12"/>
+      <c r="H79">
+        <v>600</v>
       </c>
       <c r="J79" t="s">
         <v>34</v>
@@ -2791,9 +2855,7 @@
       <c r="C80" t="s">
         <v>315</v>
       </c>
-      <c r="H80" s="11">
-        <v>10123</v>
-      </c>
+      <c r="G80" s="12"/>
       <c r="J80" t="s">
         <v>34</v>
       </c>
@@ -2808,8 +2870,9 @@
       <c r="C81" t="s">
         <v>315</v>
       </c>
+      <c r="G81" s="12"/>
       <c r="H81" s="11">
-        <v>10123</v>
+        <v>7500</v>
       </c>
       <c r="J81" t="s">
         <v>34</v>
@@ -2825,8 +2888,9 @@
       <c r="C82" t="s">
         <v>315</v>
       </c>
+      <c r="G82" s="12"/>
       <c r="H82" s="11">
-        <v>10123</v>
+        <v>7500</v>
       </c>
       <c r="J82" t="s">
         <v>34</v>
@@ -2842,8 +2906,9 @@
       <c r="C83" t="s">
         <v>315</v>
       </c>
-      <c r="H83" s="11">
-        <v>10123</v>
+      <c r="G83" s="12"/>
+      <c r="H83">
+        <v>0</v>
       </c>
       <c r="J83" t="s">
         <v>34</v>
@@ -2859,8 +2924,9 @@
       <c r="C84" t="s">
         <v>315</v>
       </c>
-      <c r="H84" s="11">
-        <v>10123</v>
+      <c r="G84" s="12"/>
+      <c r="H84">
+        <v>0</v>
       </c>
       <c r="J84" t="s">
         <v>34</v>
@@ -2876,8 +2942,9 @@
       <c r="C85" t="s">
         <v>315</v>
       </c>
+      <c r="G85" s="12"/>
       <c r="H85" s="11">
-        <v>10123</v>
+        <v>63845</v>
       </c>
       <c r="J85" t="s">
         <v>34</v>
@@ -2893,8 +2960,9 @@
       <c r="C86" t="s">
         <v>315</v>
       </c>
-      <c r="H86" s="11">
-        <v>10123</v>
+      <c r="G86" s="12"/>
+      <c r="H86">
+        <v>0</v>
       </c>
       <c r="J86" t="s">
         <v>34</v>
@@ -2910,8 +2978,9 @@
       <c r="C87" t="s">
         <v>315</v>
       </c>
-      <c r="H87" s="11">
-        <v>10123</v>
+      <c r="G87" s="12"/>
+      <c r="H87">
+        <v>0</v>
       </c>
       <c r="J87" t="s">
         <v>34</v>
@@ -2927,8 +2996,9 @@
       <c r="C88" t="s">
         <v>315</v>
       </c>
-      <c r="H88" s="11">
-        <v>10123</v>
+      <c r="G88" s="12"/>
+      <c r="H88">
+        <v>0</v>
       </c>
       <c r="J88" t="s">
         <v>34</v>
@@ -2944,8 +3014,9 @@
       <c r="C89" t="s">
         <v>315</v>
       </c>
-      <c r="H89" s="11">
-        <v>10123</v>
+      <c r="G89" s="12"/>
+      <c r="H89">
+        <v>0</v>
       </c>
       <c r="J89" t="s">
         <v>34</v>
@@ -2961,8 +3032,9 @@
       <c r="C90" t="s">
         <v>315</v>
       </c>
-      <c r="H90" s="11">
-        <v>10123</v>
+      <c r="G90" s="12"/>
+      <c r="H90">
+        <v>0</v>
       </c>
       <c r="J90" t="s">
         <v>34</v>
@@ -2978,8 +3050,9 @@
       <c r="C91" t="s">
         <v>315</v>
       </c>
-      <c r="H91" s="11">
-        <v>10123</v>
+      <c r="G91" s="12"/>
+      <c r="H91">
+        <v>0</v>
       </c>
       <c r="J91" t="s">
         <v>34</v>
@@ -2995,8 +3068,9 @@
       <c r="C92" t="s">
         <v>315</v>
       </c>
+      <c r="G92" s="12"/>
       <c r="H92" s="11">
-        <v>10123</v>
+        <v>10050</v>
       </c>
       <c r="J92" t="s">
         <v>34</v>
@@ -3012,8 +3086,9 @@
       <c r="C93" t="s">
         <v>315</v>
       </c>
+      <c r="G93" s="12"/>
       <c r="H93" s="11">
-        <v>10123</v>
+        <v>4550</v>
       </c>
       <c r="J93" t="s">
         <v>34</v>
@@ -3029,8 +3104,9 @@
       <c r="C94" t="s">
         <v>315</v>
       </c>
-      <c r="H94" s="11">
-        <v>10123</v>
+      <c r="G94" s="12"/>
+      <c r="H94">
+        <v>0</v>
       </c>
       <c r="J94" t="s">
         <v>34</v>
@@ -3046,8 +3122,9 @@
       <c r="C95" t="s">
         <v>315</v>
       </c>
+      <c r="G95" s="12"/>
       <c r="H95" s="11">
-        <v>10123</v>
+        <v>32082</v>
       </c>
       <c r="J95" t="s">
         <v>34</v>
@@ -3063,8 +3140,9 @@
       <c r="C96" t="s">
         <v>315</v>
       </c>
-      <c r="H96" s="11">
-        <v>10123</v>
+      <c r="G96" s="12"/>
+      <c r="H96">
+        <v>0</v>
       </c>
       <c r="J96" t="s">
         <v>34</v>
@@ -3080,8 +3158,9 @@
       <c r="C97" t="s">
         <v>315</v>
       </c>
-      <c r="H97" s="11">
-        <v>10123</v>
+      <c r="G97" s="12"/>
+      <c r="H97">
+        <v>0</v>
       </c>
       <c r="J97" t="s">
         <v>34</v>
@@ -3097,8 +3176,9 @@
       <c r="C98" t="s">
         <v>315</v>
       </c>
-      <c r="H98" s="11">
-        <v>10123</v>
+      <c r="G98" s="12"/>
+      <c r="H98">
+        <v>0</v>
       </c>
       <c r="J98" t="s">
         <v>34</v>
@@ -3114,8 +3194,9 @@
       <c r="C99" t="s">
         <v>315</v>
       </c>
+      <c r="G99" s="12"/>
       <c r="H99" s="11">
-        <v>10123</v>
+        <v>1120</v>
       </c>
       <c r="J99" t="s">
         <v>34</v>
@@ -3131,8 +3212,9 @@
       <c r="C100" t="s">
         <v>315</v>
       </c>
-      <c r="H100" s="11">
-        <v>10123</v>
+      <c r="G100" s="12"/>
+      <c r="H100">
+        <v>0</v>
       </c>
       <c r="J100" t="s">
         <v>34</v>
@@ -3148,8 +3230,9 @@
       <c r="C101" t="s">
         <v>315</v>
       </c>
-      <c r="H101" s="11">
-        <v>10123</v>
+      <c r="G101" s="12"/>
+      <c r="H101">
+        <v>0</v>
       </c>
       <c r="J101" t="s">
         <v>34</v>
@@ -3165,8 +3248,9 @@
       <c r="C102" t="s">
         <v>315</v>
       </c>
-      <c r="H102" s="11">
-        <v>10123</v>
+      <c r="G102" s="12"/>
+      <c r="H102">
+        <v>0</v>
       </c>
       <c r="J102" t="s">
         <v>34</v>
@@ -3182,8 +3266,9 @@
       <c r="C103" t="s">
         <v>315</v>
       </c>
-      <c r="H103" s="11">
-        <v>10123</v>
+      <c r="G103" s="12"/>
+      <c r="H103">
+        <v>0</v>
       </c>
       <c r="J103" t="s">
         <v>34</v>
@@ -3199,8 +3284,9 @@
       <c r="C104" t="s">
         <v>315</v>
       </c>
-      <c r="H104" s="11">
-        <v>10123</v>
+      <c r="G104" s="12"/>
+      <c r="H104">
+        <v>0</v>
       </c>
       <c r="J104" t="s">
         <v>34</v>
@@ -3216,8 +3302,9 @@
       <c r="C105" t="s">
         <v>315</v>
       </c>
+      <c r="G105" s="12"/>
       <c r="H105" s="11">
-        <v>10123</v>
+        <v>18640</v>
       </c>
       <c r="J105" t="s">
         <v>34</v>
@@ -3233,8 +3320,9 @@
       <c r="C106" t="s">
         <v>315</v>
       </c>
+      <c r="G106" s="12"/>
       <c r="H106" s="11">
-        <v>10123</v>
+        <v>16000</v>
       </c>
       <c r="J106" t="s">
         <v>34</v>
@@ -3250,8 +3338,9 @@
       <c r="C107" t="s">
         <v>315</v>
       </c>
+      <c r="G107" s="12"/>
       <c r="H107" s="11">
-        <v>10123</v>
+        <v>5768</v>
       </c>
       <c r="J107" t="s">
         <v>34</v>
@@ -3267,8 +3356,9 @@
       <c r="C108" t="s">
         <v>315</v>
       </c>
+      <c r="G108" s="12"/>
       <c r="H108" s="11">
-        <v>10123</v>
+        <v>21050</v>
       </c>
       <c r="J108" t="s">
         <v>34</v>
@@ -3284,8 +3374,9 @@
       <c r="C109" t="s">
         <v>315</v>
       </c>
-      <c r="H109" s="11">
-        <v>10123</v>
+      <c r="G109" s="12"/>
+      <c r="H109">
+        <v>0</v>
       </c>
       <c r="J109" t="s">
         <v>34</v>
@@ -3301,8 +3392,9 @@
       <c r="C110" t="s">
         <v>315</v>
       </c>
-      <c r="H110" s="11">
-        <v>10123</v>
+      <c r="G110" s="12"/>
+      <c r="H110">
+        <v>0</v>
       </c>
       <c r="J110" t="s">
         <v>34</v>
@@ -3318,8 +3410,9 @@
       <c r="C111" t="s">
         <v>315</v>
       </c>
+      <c r="G111" s="12"/>
       <c r="H111" s="11">
-        <v>10123</v>
+        <v>18522</v>
       </c>
       <c r="J111" t="s">
         <v>34</v>
@@ -3335,8 +3428,9 @@
       <c r="C112" t="s">
         <v>315</v>
       </c>
-      <c r="H112" s="11">
-        <v>10123</v>
+      <c r="G112" s="12"/>
+      <c r="H112">
+        <v>0</v>
       </c>
       <c r="J112" t="s">
         <v>34</v>
@@ -3352,8 +3446,9 @@
       <c r="C113" t="s">
         <v>315</v>
       </c>
-      <c r="H113" s="11">
-        <v>10123</v>
+      <c r="G113" s="12"/>
+      <c r="H113">
+        <v>0</v>
       </c>
       <c r="J113" t="s">
         <v>34</v>
@@ -3369,8 +3464,9 @@
       <c r="C114" t="s">
         <v>315</v>
       </c>
+      <c r="G114" s="12"/>
       <c r="H114" s="11">
-        <v>10123</v>
+        <v>83100</v>
       </c>
       <c r="J114" t="s">
         <v>34</v>
@@ -3386,8 +3482,9 @@
       <c r="C115" t="s">
         <v>315</v>
       </c>
-      <c r="H115" s="11">
-        <v>10123</v>
+      <c r="G115" s="12"/>
+      <c r="H115">
+        <v>0</v>
       </c>
       <c r="J115" t="s">
         <v>34</v>
@@ -3403,8 +3500,9 @@
       <c r="C116" t="s">
         <v>315</v>
       </c>
-      <c r="H116" s="11">
-        <v>10123</v>
+      <c r="G116" s="12"/>
+      <c r="H116">
+        <v>0</v>
       </c>
       <c r="J116" t="s">
         <v>34</v>
@@ -3420,8 +3518,9 @@
       <c r="C117" t="s">
         <v>315</v>
       </c>
+      <c r="G117" s="12"/>
       <c r="H117" s="11">
-        <v>10123</v>
+        <v>14000</v>
       </c>
       <c r="J117" t="s">
         <v>34</v>
@@ -3437,8 +3536,9 @@
       <c r="C118" t="s">
         <v>315</v>
       </c>
-      <c r="H118" s="11">
-        <v>10123</v>
+      <c r="G118" s="12"/>
+      <c r="H118">
+        <v>0</v>
       </c>
       <c r="J118" t="s">
         <v>34</v>
@@ -3454,8 +3554,9 @@
       <c r="C119" t="s">
         <v>315</v>
       </c>
-      <c r="H119" s="11">
-        <v>10123</v>
+      <c r="G119" s="12"/>
+      <c r="H119">
+        <v>0</v>
       </c>
       <c r="J119" t="s">
         <v>34</v>
@@ -3471,8 +3572,9 @@
       <c r="C120" t="s">
         <v>315</v>
       </c>
+      <c r="G120" s="12"/>
       <c r="H120" s="11">
-        <v>10123</v>
+        <v>1000</v>
       </c>
       <c r="J120" t="s">
         <v>34</v>
@@ -3488,8 +3590,9 @@
       <c r="C121" t="s">
         <v>315</v>
       </c>
-      <c r="H121" s="11">
-        <v>10123</v>
+      <c r="G121" s="12"/>
+      <c r="H121">
+        <v>0</v>
       </c>
       <c r="J121" t="s">
         <v>34</v>
@@ -3505,8 +3608,9 @@
       <c r="C122" t="s">
         <v>315</v>
       </c>
-      <c r="H122" s="11">
-        <v>10123</v>
+      <c r="G122" s="12"/>
+      <c r="H122">
+        <v>0</v>
       </c>
       <c r="J122" t="s">
         <v>34</v>
@@ -3522,8 +3626,9 @@
       <c r="C123" t="s">
         <v>315</v>
       </c>
-      <c r="H123" s="11">
-        <v>10123</v>
+      <c r="G123" s="12"/>
+      <c r="H123">
+        <v>0</v>
       </c>
       <c r="J123" t="s">
         <v>34</v>
@@ -3539,8 +3644,9 @@
       <c r="C124" t="s">
         <v>315</v>
       </c>
-      <c r="H124" s="11">
-        <v>10123</v>
+      <c r="G124" s="12"/>
+      <c r="H124">
+        <v>0</v>
       </c>
       <c r="J124" t="s">
         <v>34</v>
@@ -3556,8 +3662,9 @@
       <c r="C125" t="s">
         <v>315</v>
       </c>
-      <c r="H125" s="11">
-        <v>10123</v>
+      <c r="G125" s="12"/>
+      <c r="H125">
+        <v>0</v>
       </c>
       <c r="J125" t="s">
         <v>34</v>
@@ -3573,8 +3680,9 @@
       <c r="C126" t="s">
         <v>315</v>
       </c>
-      <c r="H126" s="11">
-        <v>10123</v>
+      <c r="G126" s="12"/>
+      <c r="H126">
+        <v>0</v>
       </c>
       <c r="J126" t="s">
         <v>34</v>
@@ -3590,8 +3698,9 @@
       <c r="C127" t="s">
         <v>315</v>
       </c>
-      <c r="H127" s="11">
-        <v>10123</v>
+      <c r="G127" s="12"/>
+      <c r="H127">
+        <v>0</v>
       </c>
       <c r="J127" t="s">
         <v>34</v>
@@ -3607,8 +3716,9 @@
       <c r="C128" t="s">
         <v>315</v>
       </c>
-      <c r="H128" s="11">
-        <v>10123</v>
+      <c r="G128" s="12"/>
+      <c r="H128">
+        <v>0</v>
       </c>
       <c r="J128" t="s">
         <v>34</v>
@@ -3624,8 +3734,9 @@
       <c r="C129" t="s">
         <v>315</v>
       </c>
-      <c r="H129" s="11">
-        <v>10123</v>
+      <c r="G129" s="12"/>
+      <c r="H129">
+        <v>0</v>
       </c>
       <c r="J129" t="s">
         <v>34</v>
@@ -3641,8 +3752,9 @@
       <c r="C130" t="s">
         <v>315</v>
       </c>
-      <c r="H130" s="11">
-        <v>10123</v>
+      <c r="G130" s="12"/>
+      <c r="H130">
+        <v>0</v>
       </c>
       <c r="J130" t="s">
         <v>34</v>
@@ -3658,8 +3770,9 @@
       <c r="C131" t="s">
         <v>315</v>
       </c>
+      <c r="G131" s="12"/>
       <c r="H131" s="11">
-        <v>10123</v>
+        <v>27433</v>
       </c>
       <c r="J131" t="s">
         <v>34</v>
@@ -3675,8 +3788,9 @@
       <c r="C132" t="s">
         <v>315</v>
       </c>
-      <c r="H132" s="11">
-        <v>10123</v>
+      <c r="G132" s="12"/>
+      <c r="H132">
+        <v>250</v>
       </c>
       <c r="J132" t="s">
         <v>34</v>
@@ -3692,8 +3806,9 @@
       <c r="C133" t="s">
         <v>315</v>
       </c>
+      <c r="G133" s="12"/>
       <c r="H133" s="11">
-        <v>10123</v>
+        <v>3064</v>
       </c>
       <c r="J133" t="s">
         <v>34</v>
@@ -3709,8 +3824,9 @@
       <c r="C134" t="s">
         <v>315</v>
       </c>
-      <c r="H134" s="11">
-        <v>10123</v>
+      <c r="G134" s="12"/>
+      <c r="H134">
+        <v>0</v>
       </c>
       <c r="J134" t="s">
         <v>34</v>
@@ -3726,8 +3842,9 @@
       <c r="C135" t="s">
         <v>315</v>
       </c>
-      <c r="H135" s="11">
-        <v>10123</v>
+      <c r="G135" s="12"/>
+      <c r="H135">
+        <v>0</v>
       </c>
       <c r="J135" t="s">
         <v>34</v>
@@ -3743,8 +3860,9 @@
       <c r="C136" t="s">
         <v>315</v>
       </c>
-      <c r="H136" s="11">
-        <v>10123</v>
+      <c r="G136" s="12"/>
+      <c r="H136">
+        <v>0</v>
       </c>
       <c r="J136" t="s">
         <v>34</v>
@@ -3760,8 +3878,9 @@
       <c r="C137" t="s">
         <v>315</v>
       </c>
-      <c r="H137" s="11">
-        <v>10123</v>
+      <c r="G137" s="12"/>
+      <c r="H137">
+        <v>500</v>
       </c>
       <c r="J137" t="s">
         <v>34</v>
@@ -3777,8 +3896,9 @@
       <c r="C138" t="s">
         <v>315</v>
       </c>
-      <c r="H138" s="11">
-        <v>10123</v>
+      <c r="G138" s="12"/>
+      <c r="H138">
+        <v>0</v>
       </c>
       <c r="J138" t="s">
         <v>34</v>
@@ -3794,8 +3914,9 @@
       <c r="C139" t="s">
         <v>315</v>
       </c>
+      <c r="G139" s="12"/>
       <c r="H139" s="11">
-        <v>10123</v>
+        <v>28270</v>
       </c>
       <c r="J139" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Added real Degree Days to Other Data spreadsheet.
</commit_message>
<xml_diff>
--- a/data/Other_Building_Data.xlsx
+++ b/data/Other_Building_Data.xlsx
@@ -31,9 +31,6 @@
     <t>Site ID</t>
   </si>
   <si>
-    <t>Other Building Information</t>
-  </si>
-  <si>
     <t>Site Name</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     <t>dd_site</t>
   </si>
   <si>
-    <t>Information About Fuels</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
     <t>PAFA</t>
   </si>
   <si>
-    <t>The last 36 months are accurate (Sep-2014 - Aug-2017)</t>
-  </si>
-  <si>
     <t>btu_per_unit</t>
   </si>
   <si>
@@ -977,6 +968,39 @@
   </si>
   <si>
     <t>site_id</t>
+  </si>
+  <si>
+    <t>Make sure the "Month" header row starts on row 4.</t>
+  </si>
+  <si>
+    <r>
+      <t>Other Building Information (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>make sure "Site ID" header rows starts on Row 3)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Information About Fuels </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(make sure "Fuel" header rows starts on Row 3)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -987,7 +1011,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1020,6 +1044,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1408,9 +1439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L139"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1427,7 +1456,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -1435,2495 +1464,2496 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="7" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="11">
         <v>49210</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="11">
         <v>49210</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="11">
         <v>234412</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="11">
         <v>57047</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="11">
         <v>64699</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="11">
         <v>74654</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11">
         <v>60642</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="11">
         <v>13608</v>
       </c>
       <c r="J12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="11">
         <v>24496</v>
       </c>
       <c r="J13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="11">
         <v>81654</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="11">
         <v>57154</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="11">
         <v>99880</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="11">
         <v>137524</v>
       </c>
       <c r="J17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G18" s="12"/>
       <c r="H18" s="11">
         <v>32832</v>
       </c>
       <c r="J18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G19" s="12"/>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C20" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="11">
         <v>43996</v>
       </c>
       <c r="J21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="11">
         <v>103200</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G23" s="12"/>
       <c r="H23" s="11">
         <v>113306</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="11">
         <v>156362</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C25" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="11">
         <v>101069</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="11">
         <v>216884</v>
       </c>
       <c r="J26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C27" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="11">
         <v>64408</v>
       </c>
       <c r="J27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G28" s="12"/>
       <c r="H28" s="11">
         <v>64458</v>
       </c>
       <c r="J28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G29" s="12"/>
       <c r="H29" s="11">
         <v>62982</v>
       </c>
       <c r="J29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G30" s="12"/>
       <c r="H30" s="11">
         <v>22200</v>
       </c>
       <c r="J30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C31" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G31" s="12"/>
       <c r="H31" s="11">
         <v>65259</v>
       </c>
       <c r="J31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G32" s="12"/>
       <c r="H32" s="11">
         <v>63761</v>
       </c>
       <c r="J32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G33" s="12"/>
       <c r="H33" s="11">
         <v>30856</v>
       </c>
       <c r="J33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G34" s="12"/>
       <c r="H34" s="11">
         <v>63455</v>
       </c>
       <c r="J34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G35" s="12"/>
       <c r="H35" s="11">
         <v>68272</v>
       </c>
       <c r="J35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B36" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C36" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G36" s="12"/>
       <c r="H36" s="11">
         <v>63532</v>
       </c>
       <c r="J36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C37" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G37" s="12"/>
       <c r="J37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="11">
         <v>63532</v>
       </c>
       <c r="J38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G39" s="12"/>
       <c r="H39" s="11">
         <v>74589</v>
       </c>
       <c r="J39" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C40" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G40" s="12"/>
       <c r="J40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C41" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G41" s="12"/>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="J41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C42" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="J42" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" t="s">
+        <v>312</v>
+      </c>
+      <c r="D43" t="s">
         <v>10</v>
       </c>
-      <c r="B43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" t="s">
-        <v>315</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>11</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>12</v>
-      </c>
-      <c r="F43" t="s">
-        <v>13</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="11">
         <v>6718</v>
       </c>
       <c r="J43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="11">
         <v>2350</v>
       </c>
       <c r="J44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C46" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="11">
         <v>1800</v>
       </c>
       <c r="J46" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C47" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G47" s="12"/>
       <c r="H47">
         <v>242</v>
       </c>
       <c r="J47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B48" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="11">
         <v>2268</v>
       </c>
       <c r="J48" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="11">
         <v>35500</v>
       </c>
       <c r="J49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C50" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="J50" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G51" s="12"/>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="J51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C52" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="11">
         <v>13500</v>
       </c>
       <c r="J52" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G53" s="12"/>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="J53" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C54" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G54" s="12"/>
       <c r="H54" s="11">
         <v>2350</v>
       </c>
       <c r="J54" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G55" s="12"/>
       <c r="H55" s="11">
         <v>11188</v>
       </c>
       <c r="J55" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B56" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G56" s="12"/>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="J56" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G57" s="12"/>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="J57" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C58" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G58" s="12"/>
       <c r="H58" s="11">
         <v>5600</v>
       </c>
       <c r="J58" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C59" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G59" s="12"/>
       <c r="H59" s="11">
         <v>3742</v>
       </c>
       <c r="J59" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G60" s="12"/>
       <c r="H60" s="11">
         <v>34500</v>
       </c>
       <c r="J60" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C61" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G61" s="12"/>
       <c r="H61" s="11">
         <v>44892</v>
       </c>
       <c r="J61" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C62" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G62" s="12"/>
       <c r="H62">
         <v>0</v>
       </c>
       <c r="J62" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B63" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C63" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G63" s="12"/>
       <c r="H63">
         <v>440</v>
       </c>
       <c r="J63" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C64" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G64" s="12"/>
       <c r="H64" s="11">
         <v>1392</v>
       </c>
       <c r="J64" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G65" s="12"/>
       <c r="H65" s="11">
         <v>2620</v>
       </c>
       <c r="J65" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C66" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G66" s="12"/>
       <c r="H66" s="11">
         <v>1180</v>
       </c>
       <c r="J66" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C67" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G67" s="12"/>
       <c r="H67" s="11">
         <v>11175</v>
       </c>
       <c r="J67" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B68" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C68" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G68" s="12"/>
       <c r="H68">
         <v>0</v>
       </c>
       <c r="J68" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B69" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C69" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G69" s="12"/>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="J69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B70" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C70" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G70" s="12"/>
       <c r="H70">
         <v>0</v>
       </c>
       <c r="J70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C71" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G71" s="12"/>
       <c r="H71">
         <v>0</v>
       </c>
       <c r="J71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B72" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C72" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G72" s="12"/>
       <c r="H72" s="11">
         <v>118800</v>
       </c>
       <c r="J72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B73" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C73" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G73" s="12"/>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="J73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C74" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G74" s="12"/>
       <c r="J74" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B75" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C75" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G75" s="12"/>
       <c r="H75">
         <v>0</v>
       </c>
       <c r="J75" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C76" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G76" s="12"/>
       <c r="H76">
         <v>0</v>
       </c>
       <c r="J76" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C77" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G77" s="12"/>
       <c r="H77">
         <v>0</v>
       </c>
       <c r="J77" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B78" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C78" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78">
         <v>0</v>
       </c>
       <c r="J78" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B79" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C79" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G79" s="12"/>
       <c r="H79">
         <v>600</v>
       </c>
       <c r="J79" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B80" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C80" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G80" s="12"/>
       <c r="J80" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B81" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C81" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G81" s="12"/>
       <c r="H81" s="11">
         <v>7500</v>
       </c>
       <c r="J81" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B82" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C82" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G82" s="12"/>
       <c r="H82" s="11">
         <v>7500</v>
       </c>
       <c r="J82" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B83" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C83" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G83" s="12"/>
       <c r="H83">
         <v>0</v>
       </c>
       <c r="J83" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B84" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C84" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G84" s="12"/>
       <c r="H84">
         <v>0</v>
       </c>
       <c r="J84" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B85" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C85" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G85" s="12"/>
       <c r="H85" s="11">
         <v>63845</v>
       </c>
       <c r="J85" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B86" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C86" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G86" s="12"/>
       <c r="H86">
         <v>0</v>
       </c>
       <c r="J86" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B87" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C87" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G87" s="12"/>
       <c r="H87">
         <v>0</v>
       </c>
       <c r="J87" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B88" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C88" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G88" s="12"/>
       <c r="H88">
         <v>0</v>
       </c>
       <c r="J88" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B89" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C89" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G89" s="12"/>
       <c r="H89">
         <v>0</v>
       </c>
       <c r="J89" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B90" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C90" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G90" s="12"/>
       <c r="H90">
         <v>0</v>
       </c>
       <c r="J90" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B91" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C91" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G91" s="12"/>
       <c r="H91">
         <v>0</v>
       </c>
       <c r="J91" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B92" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C92" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G92" s="12"/>
       <c r="H92" s="11">
         <v>10050</v>
       </c>
       <c r="J92" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B93" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C93" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G93" s="12"/>
       <c r="H93" s="11">
         <v>4550</v>
       </c>
       <c r="J93" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B94" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C94" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G94" s="12"/>
       <c r="H94">
         <v>0</v>
       </c>
       <c r="J94" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B95" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C95" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G95" s="12"/>
       <c r="H95" s="11">
         <v>32082</v>
       </c>
       <c r="J95" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B96" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C96" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G96" s="12"/>
       <c r="H96">
         <v>0</v>
       </c>
       <c r="J96" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B97" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C97" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G97" s="12"/>
       <c r="H97">
         <v>0</v>
       </c>
       <c r="J97" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B98" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C98" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G98" s="12"/>
       <c r="H98">
         <v>0</v>
       </c>
       <c r="J98" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B99" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C99" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G99" s="12"/>
       <c r="H99" s="11">
         <v>1120</v>
       </c>
       <c r="J99" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B100" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C100" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G100" s="12"/>
       <c r="H100">
         <v>0</v>
       </c>
       <c r="J100" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B101" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C101" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G101" s="12"/>
       <c r="H101">
         <v>0</v>
       </c>
       <c r="J101" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B102" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C102" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G102" s="12"/>
       <c r="H102">
         <v>0</v>
       </c>
       <c r="J102" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B103" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C103" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G103" s="12"/>
       <c r="H103">
         <v>0</v>
       </c>
       <c r="J103" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B104" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C104" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G104" s="12"/>
       <c r="H104">
         <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B105" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C105" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G105" s="12"/>
       <c r="H105" s="11">
         <v>18640</v>
       </c>
       <c r="J105" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B106" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C106" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G106" s="12"/>
       <c r="H106" s="11">
         <v>16000</v>
       </c>
       <c r="J106" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B107" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C107" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G107" s="12"/>
       <c r="H107" s="11">
         <v>5768</v>
       </c>
       <c r="J107" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B108" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C108" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G108" s="12"/>
       <c r="H108" s="11">
         <v>21050</v>
       </c>
       <c r="J108" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B109" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C109" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G109" s="12"/>
       <c r="H109">
         <v>0</v>
       </c>
       <c r="J109" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B110" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C110" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G110" s="12"/>
       <c r="H110">
         <v>0</v>
       </c>
       <c r="J110" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B111" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C111" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G111" s="12"/>
       <c r="H111" s="11">
         <v>18522</v>
       </c>
       <c r="J111" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B112" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C112" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G112" s="12"/>
       <c r="H112">
         <v>0</v>
       </c>
       <c r="J112" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B113" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C113" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G113" s="12"/>
       <c r="H113">
         <v>0</v>
       </c>
       <c r="J113" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B114" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C114" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G114" s="12"/>
       <c r="H114" s="11">
         <v>83100</v>
       </c>
       <c r="J114" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B115" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C115" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G115" s="12"/>
       <c r="H115">
         <v>0</v>
       </c>
       <c r="J115" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B116" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C116" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G116" s="12"/>
       <c r="H116">
         <v>0</v>
       </c>
       <c r="J116" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B117" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C117" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G117" s="12"/>
       <c r="H117" s="11">
         <v>14000</v>
       </c>
       <c r="J117" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B118" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C118" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G118" s="12"/>
       <c r="H118">
         <v>0</v>
       </c>
       <c r="J118" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B119" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C119" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G119" s="12"/>
       <c r="H119">
         <v>0</v>
       </c>
       <c r="J119" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B120" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C120" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G120" s="12"/>
       <c r="H120" s="11">
         <v>1000</v>
       </c>
       <c r="J120" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B121" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C121" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G121" s="12"/>
       <c r="H121">
         <v>0</v>
       </c>
       <c r="J121" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B122" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C122" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G122" s="12"/>
       <c r="H122">
         <v>0</v>
       </c>
       <c r="J122" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B123" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C123" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G123" s="12"/>
       <c r="H123">
         <v>0</v>
       </c>
       <c r="J123" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B124" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C124" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G124" s="12"/>
       <c r="H124">
         <v>0</v>
       </c>
       <c r="J124" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B125" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C125" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G125" s="12"/>
       <c r="H125">
         <v>0</v>
       </c>
       <c r="J125" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B126" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C126" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G126" s="12"/>
       <c r="H126">
         <v>0</v>
       </c>
       <c r="J126" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B127" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C127" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G127" s="12"/>
       <c r="H127">
         <v>0</v>
       </c>
       <c r="J127" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B128" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C128" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G128" s="12"/>
       <c r="H128">
         <v>0</v>
       </c>
       <c r="J128" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B129" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C129" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G129" s="12"/>
       <c r="H129">
         <v>0</v>
       </c>
       <c r="J129" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B130" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C130" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G130" s="12"/>
       <c r="H130">
         <v>0</v>
       </c>
       <c r="J130" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B131" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C131" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G131" s="12"/>
       <c r="H131" s="11">
         <v>27433</v>
       </c>
       <c r="J131" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B132" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C132" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G132" s="12"/>
       <c r="H132">
         <v>250</v>
       </c>
       <c r="J132" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B133" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C133" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G133" s="12"/>
       <c r="H133" s="11">
         <v>3064</v>
       </c>
       <c r="J133" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B134" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C134" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G134" s="12"/>
       <c r="H134">
         <v>0</v>
       </c>
       <c r="J134" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B135" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C135" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G135" s="12"/>
       <c r="H135">
         <v>0</v>
       </c>
       <c r="J135" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B136" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C136" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G136" s="12"/>
       <c r="H136">
         <v>0</v>
       </c>
       <c r="J136" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B137" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C137" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G137" s="12"/>
       <c r="H137">
         <v>500</v>
       </c>
       <c r="J137" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B138" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C138" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G138" s="12"/>
       <c r="H138">
         <v>0</v>
       </c>
       <c r="J138" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B139" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C139" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G139" s="12"/>
       <c r="H139" s="11">
         <v>28270</v>
       </c>
       <c r="J139" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="A21" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -3932,1070 +3962,1159 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B145"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
-        <v>39083</v>
+        <v>38718</v>
       </c>
       <c r="B5">
-        <v>1902</v>
+        <v>2699</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
-        <v>39114</v>
+        <v>38749</v>
       </c>
       <c r="B6">
-        <v>1689</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
-        <v>39142</v>
+        <v>38777</v>
       </c>
       <c r="B7">
-        <v>1390</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
-        <v>39173</v>
+        <v>38808</v>
       </c>
       <c r="B8">
-        <v>689</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
-        <v>39203</v>
+        <v>38838</v>
       </c>
       <c r="B9">
-        <v>367</v>
+        <v>473</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
-        <v>39234</v>
+        <v>38869</v>
       </c>
       <c r="B10">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
-        <v>39264</v>
+        <v>38899</v>
       </c>
       <c r="B11">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
-        <v>39295</v>
+        <v>38930</v>
       </c>
       <c r="B12">
-        <v>169</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
-        <v>39326</v>
+        <v>38961</v>
       </c>
       <c r="B13">
-        <v>568</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
-        <v>39356</v>
+        <v>38991</v>
       </c>
       <c r="B14">
-        <v>1232</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
-        <v>39387</v>
+        <v>39022</v>
       </c>
       <c r="B15">
-        <v>1825</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
-        <v>39417</v>
+        <v>39052</v>
       </c>
       <c r="B16">
-        <v>2245</v>
+        <v>2074</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
-        <v>39448</v>
+        <v>39083</v>
       </c>
       <c r="B17">
-        <v>2302</v>
+        <v>2218</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
-        <v>39479</v>
+        <v>39114</v>
       </c>
       <c r="B18">
-        <v>1797</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
-        <v>39508</v>
+        <v>39142</v>
       </c>
       <c r="B19">
-        <v>2084</v>
+        <v>2215</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
-        <v>39539</v>
+        <v>39173</v>
       </c>
       <c r="B20">
-        <v>863</v>
+        <v>821</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
-        <v>39569</v>
+        <v>39203</v>
       </c>
       <c r="B21">
-        <v>448</v>
+        <v>434</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
-        <v>39600</v>
+        <v>39234</v>
       </c>
       <c r="B22">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
-        <v>39630</v>
+        <v>39264</v>
       </c>
       <c r="B23">
-        <v>86</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
-        <v>39661</v>
+        <v>39295</v>
       </c>
       <c r="B24">
-        <v>248</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
-        <v>39692</v>
+        <v>39326</v>
       </c>
       <c r="B25">
-        <v>574</v>
+        <v>537</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
-        <v>39722</v>
+        <v>39356</v>
       </c>
       <c r="B26">
-        <v>1222</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
-        <v>39753</v>
+        <v>39387</v>
       </c>
       <c r="B27">
-        <v>1658</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
-        <v>39783</v>
+        <v>39417</v>
       </c>
       <c r="B28">
-        <v>1747</v>
+        <v>2117</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
-        <v>39814</v>
+        <v>39448</v>
       </c>
       <c r="B29">
-        <v>2196</v>
+        <v>2298</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
-        <v>39845</v>
+        <v>39479</v>
       </c>
       <c r="B30">
-        <v>1804</v>
+        <v>2055</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
-        <v>39873</v>
+        <v>39508</v>
       </c>
       <c r="B31">
-        <v>1524</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
-        <v>39904</v>
+        <v>39539</v>
       </c>
       <c r="B32">
-        <v>828</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
-        <v>39934</v>
+        <v>39569</v>
       </c>
       <c r="B33">
-        <v>298</v>
+        <v>467</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
-        <v>39965</v>
+        <v>39600</v>
       </c>
       <c r="B34">
-        <v>208</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
-        <v>39995</v>
+        <v>39630</v>
       </c>
       <c r="B35">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
-        <v>40026</v>
+        <v>39661</v>
       </c>
       <c r="B36">
-        <v>349</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
-        <v>40057</v>
+        <v>39692</v>
       </c>
       <c r="B37">
-        <v>683</v>
+        <v>549</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
-        <v>40087</v>
+        <v>39722</v>
       </c>
       <c r="B38">
-        <v>1047</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
-        <v>40118</v>
+        <v>39753</v>
       </c>
       <c r="B39">
-        <v>1649</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
-        <v>40148</v>
+        <v>39783</v>
       </c>
       <c r="B40">
-        <v>2058</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
-        <v>40179</v>
+        <v>39814</v>
       </c>
       <c r="B41">
-        <v>1902</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
-        <v>40210</v>
+        <v>39845</v>
       </c>
       <c r="B42">
-        <v>1689</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
-        <v>40238</v>
+        <v>39873</v>
       </c>
       <c r="B43">
-        <v>1390</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
-        <v>40269</v>
+        <v>39904</v>
       </c>
       <c r="B44">
-        <v>689</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="10">
-        <v>40299</v>
+        <v>39934</v>
       </c>
       <c r="B45">
-        <v>367</v>
+        <v>416</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="10">
-        <v>40330</v>
+        <v>39965</v>
       </c>
       <c r="B46">
-        <v>197</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="10">
-        <v>40360</v>
+        <v>39995</v>
       </c>
       <c r="B47">
-        <v>134</v>
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="10">
-        <v>40391</v>
+        <v>40026</v>
       </c>
       <c r="B48">
-        <v>169</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
-        <v>40422</v>
+        <v>40057</v>
       </c>
       <c r="B49">
-        <v>568</v>
+        <v>493</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
-        <v>40452</v>
+        <v>40087</v>
       </c>
       <c r="B50">
-        <v>1232</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
-        <v>40483</v>
+        <v>40118</v>
       </c>
       <c r="B51">
-        <v>1825</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
-        <v>40513</v>
+        <v>40148</v>
       </c>
       <c r="B52">
-        <v>2245</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
-        <v>40544</v>
+        <v>40179</v>
       </c>
       <c r="B53">
-        <v>2302</v>
+        <v>2439</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
-        <v>40575</v>
+        <v>40210</v>
       </c>
       <c r="B54">
-        <v>1797</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
-        <v>40603</v>
+        <v>40238</v>
       </c>
       <c r="B55">
-        <v>2084</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
-        <v>40634</v>
+        <v>40269</v>
       </c>
       <c r="B56">
-        <v>863</v>
+        <v>765</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="10">
-        <v>40664</v>
+        <v>40299</v>
       </c>
       <c r="B57">
-        <v>448</v>
+        <v>347</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="10">
-        <v>40695</v>
+        <v>40330</v>
       </c>
       <c r="B58">
-        <v>135</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="10">
-        <v>40725</v>
+        <v>40360</v>
       </c>
       <c r="B59">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="10">
-        <v>40756</v>
+        <v>40391</v>
       </c>
       <c r="B60">
-        <v>248</v>
+        <v>191</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="10">
-        <v>40787</v>
+        <v>40422</v>
       </c>
       <c r="B61">
-        <v>574</v>
+        <v>535</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="10">
-        <v>40817</v>
+        <v>40452</v>
       </c>
       <c r="B62">
-        <v>1222</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
-        <v>40848</v>
+        <v>40483</v>
       </c>
       <c r="B63">
-        <v>1658</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="10">
-        <v>40878</v>
+        <v>40513</v>
       </c>
       <c r="B64">
-        <v>1747</v>
+        <v>2567</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="10">
-        <v>40909</v>
+        <v>40544</v>
       </c>
       <c r="B65">
-        <v>2196</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="10">
-        <v>40940</v>
+        <v>40575</v>
       </c>
       <c r="B66">
-        <v>1804</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="10">
-        <v>40969</v>
+        <v>40603</v>
       </c>
       <c r="B67">
-        <v>1524</v>
+        <v>1789</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="10">
-        <v>41000</v>
+        <v>40634</v>
       </c>
       <c r="B68">
-        <v>828</v>
+        <v>995</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="10">
-        <v>41030</v>
+        <v>40664</v>
       </c>
       <c r="B69">
-        <v>298</v>
+        <v>403</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
-        <v>41061</v>
+        <v>40695</v>
       </c>
       <c r="B70">
-        <v>208</v>
+        <v>146</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="10">
-        <v>41091</v>
+        <v>40725</v>
       </c>
       <c r="B71">
-        <v>151</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="10">
-        <v>41122</v>
+        <v>40756</v>
       </c>
       <c r="B72">
-        <v>349</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="10">
-        <v>41153</v>
+        <v>40787</v>
       </c>
       <c r="B73">
-        <v>683</v>
+        <v>481</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="10">
-        <v>41183</v>
+        <v>40817</v>
       </c>
       <c r="B74">
-        <v>1047</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="10">
-        <v>41214</v>
+        <v>40848</v>
       </c>
       <c r="B75">
-        <v>1649</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="10">
-        <v>41244</v>
+        <v>40878</v>
       </c>
       <c r="B76">
-        <v>2058</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="10">
-        <v>41275</v>
+        <v>40909</v>
       </c>
       <c r="B77">
-        <v>1902</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="10">
-        <v>41306</v>
+        <v>40940</v>
       </c>
       <c r="B78">
-        <v>1689</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="10">
-        <v>41334</v>
+        <v>40969</v>
       </c>
       <c r="B79">
-        <v>1390</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="10">
-        <v>41365</v>
+        <v>41000</v>
       </c>
       <c r="B80">
-        <v>689</v>
+        <v>842</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="10">
-        <v>41395</v>
+        <v>41030</v>
       </c>
       <c r="B81">
-        <v>367</v>
+        <v>529</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="10">
-        <v>41426</v>
+        <v>41061</v>
       </c>
       <c r="B82">
-        <v>197</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="10">
-        <v>41456</v>
+        <v>41091</v>
       </c>
       <c r="B83">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="10">
-        <v>41487</v>
+        <v>41122</v>
       </c>
       <c r="B84">
-        <v>169</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="10">
-        <v>41518</v>
+        <v>41153</v>
       </c>
       <c r="B85">
-        <v>568</v>
+        <v>582</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="10">
-        <v>41548</v>
+        <v>41183</v>
       </c>
       <c r="B86">
-        <v>1232</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="10">
-        <v>41579</v>
+        <v>41214</v>
       </c>
       <c r="B87">
-        <v>1825</v>
+        <v>2211</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="10">
-        <v>41609</v>
+        <v>41244</v>
       </c>
       <c r="B88">
-        <v>2245</v>
+        <v>2548</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="10">
-        <v>41640</v>
+        <v>41275</v>
       </c>
       <c r="B89">
-        <v>2302</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="10">
-        <v>41671</v>
+        <v>41306</v>
       </c>
       <c r="B90">
-        <v>1797</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="10">
-        <v>41699</v>
+        <v>41334</v>
       </c>
       <c r="B91">
-        <v>2084</v>
+        <v>1792</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="10">
-        <v>41730</v>
+        <v>41365</v>
       </c>
       <c r="B92">
-        <v>863</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="10">
-        <v>41760</v>
+        <v>41395</v>
       </c>
       <c r="B93">
-        <v>448</v>
+        <v>650</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="10">
-        <v>41791</v>
+        <v>41426</v>
       </c>
       <c r="B94">
-        <v>135</v>
+        <v>73</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
-        <v>41821</v>
+        <v>41456</v>
       </c>
       <c r="B95">
-        <v>86</v>
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
-        <v>41852</v>
+        <v>41487</v>
       </c>
       <c r="B96">
-        <v>248</v>
+        <v>195</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
-        <v>41883</v>
+        <v>41518</v>
       </c>
       <c r="B97">
-        <v>574</v>
+        <v>634</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
-        <v>41913</v>
+        <v>41548</v>
       </c>
       <c r="B98">
-        <v>1222</v>
+        <v>891</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="10">
-        <v>41944</v>
+        <v>41579</v>
       </c>
       <c r="B99">
-        <v>1658</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
-        <v>41974</v>
+        <v>41609</v>
       </c>
       <c r="B100">
-        <v>1747</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
-        <v>42005</v>
+        <v>41640</v>
       </c>
       <c r="B101">
-        <v>2196</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="10">
-        <v>42036</v>
+        <v>41671</v>
       </c>
       <c r="B102">
-        <v>1804</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="10">
-        <v>42064</v>
+        <v>41699</v>
       </c>
       <c r="B103">
-        <v>1524</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="10">
-        <v>42095</v>
+        <v>41730</v>
       </c>
       <c r="B104">
-        <v>828</v>
+        <v>928</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="10">
-        <v>42125</v>
+        <v>41760</v>
       </c>
       <c r="B105">
-        <v>298</v>
+        <v>422</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="10">
-        <v>42156</v>
+        <v>41791</v>
       </c>
       <c r="B106">
-        <v>208</v>
+        <v>196</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="10">
-        <v>42186</v>
+        <v>41821</v>
       </c>
       <c r="B107">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
-        <v>42217</v>
+        <v>41852</v>
       </c>
       <c r="B108">
-        <v>349</v>
+        <v>188</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="10">
-        <v>42248</v>
+        <v>41883</v>
       </c>
       <c r="B109">
-        <v>683</v>
+        <v>556</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="10">
-        <v>42278</v>
+        <v>41913</v>
       </c>
       <c r="B110">
-        <v>1047</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="10">
-        <v>42309</v>
+        <v>41944</v>
       </c>
       <c r="B111">
-        <v>1649</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="10">
-        <v>42339</v>
+        <v>41974</v>
       </c>
       <c r="B112">
-        <v>2058</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="10">
-        <v>42370</v>
+        <v>42005</v>
       </c>
       <c r="B113">
-        <v>1902</v>
+        <v>2208</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="10">
-        <v>42401</v>
+        <v>42036</v>
       </c>
       <c r="B114">
-        <v>1689</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="10">
-        <v>42430</v>
+        <v>42064</v>
       </c>
       <c r="B115">
-        <v>1390</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="10">
-        <v>42461</v>
+        <v>42095</v>
       </c>
       <c r="B116">
-        <v>689</v>
+        <v>842</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="10">
-        <v>42491</v>
+        <v>42125</v>
       </c>
       <c r="B117">
-        <v>367</v>
+        <v>302</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="10">
-        <v>42522</v>
+        <v>42156</v>
       </c>
       <c r="B118">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="10">
-        <v>42552</v>
+        <v>42186</v>
       </c>
       <c r="B119">
-        <v>134</v>
+        <v>106</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="10">
-        <v>42583</v>
+        <v>42217</v>
       </c>
       <c r="B120">
-        <v>169</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="10">
-        <v>42614</v>
+        <v>42248</v>
       </c>
       <c r="B121">
-        <v>568</v>
+        <v>675</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="10">
-        <v>42644</v>
+        <v>42278</v>
       </c>
       <c r="B122">
-        <v>1232</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="10">
-        <v>42675</v>
+        <v>42309</v>
       </c>
       <c r="B123">
-        <v>1825</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="10">
-        <v>42705</v>
+        <v>42339</v>
       </c>
       <c r="B124">
-        <v>2245</v>
+        <v>2075</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="10">
-        <v>42736</v>
+        <v>42370</v>
       </c>
       <c r="B125">
-        <v>2302</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="10">
-        <v>42767</v>
+        <v>42401</v>
       </c>
       <c r="B126">
-        <v>1797</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="10">
-        <v>42795</v>
+        <v>42430</v>
       </c>
       <c r="B127">
-        <v>2084</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="10">
-        <v>42826</v>
+        <v>42461</v>
       </c>
       <c r="B128">
-        <v>863</v>
+        <v>689</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="10">
-        <v>42856</v>
+        <v>42491</v>
       </c>
       <c r="B129">
-        <v>448</v>
+        <v>367</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="10">
-        <v>42887</v>
+        <v>42522</v>
       </c>
       <c r="B130">
-        <v>135</v>
+        <v>197</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="10">
-        <v>42917</v>
+        <v>42552</v>
       </c>
       <c r="B131">
-        <v>86</v>
+        <v>134</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="10">
+        <v>42583</v>
+      </c>
+      <c r="B132">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="10">
+        <v>42614</v>
+      </c>
+      <c r="B133">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="10">
+        <v>42644</v>
+      </c>
+      <c r="B134">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="10">
+        <v>42675</v>
+      </c>
+      <c r="B135">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="10">
+        <v>42705</v>
+      </c>
+      <c r="B136">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="10">
+        <v>42736</v>
+      </c>
+      <c r="B137">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="10">
+        <v>42767</v>
+      </c>
+      <c r="B138">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="10">
+        <v>42795</v>
+      </c>
+      <c r="B139">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="10">
+        <v>42826</v>
+      </c>
+      <c r="B140">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="10">
+        <v>42856</v>
+      </c>
+      <c r="B141">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="10">
+        <v>42887</v>
+      </c>
+      <c r="B142">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="10">
+        <v>42917</v>
+      </c>
+      <c r="B143">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="10">
         <v>42948</v>
       </c>
-      <c r="B132">
+      <c r="B144">
         <v>248</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="10"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="10"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="10"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="10"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="10"/>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="10">
+        <v>42979</v>
+      </c>
+      <c r="B145">
+        <v>524</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5007,9 +5126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5019,38 +5136,38 @@
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2">
         <v>102000</v>
@@ -5058,10 +5175,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2">
         <v>3412</v>
@@ -5069,10 +5186,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>135000</v>
@@ -5080,10 +5197,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2">
         <v>1000000</v>
@@ -5091,10 +5208,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2">
         <v>1194000</v>
@@ -5102,10 +5219,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
         <v>39</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
       </c>
       <c r="C10" s="2">
         <v>1194</v>

</xml_diff>